<commit_message>
Add new features, fix bugs
</commit_message>
<xml_diff>
--- a/mysite/DB6_Storage.xlsx
+++ b/mysite/DB6_Storage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSC\django-wms-skw\mysite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\django-wms\mysite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0B16DD-08C4-4FAE-BF56-0AB753E3BCD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53D4D4B-8475-4074-A433-67564C0E52AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dataset!$F$1:$J$1031</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dataset!$F$1:$J$1046</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2291" uniqueCount="1845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2295" uniqueCount="1847">
   <si>
     <t>storage_id</t>
   </si>
@@ -3843,6 +3843,12 @@
   </si>
   <si>
     <t>2019-10-08 19:37:04</t>
+  </si>
+  <si>
+    <t>2019-10-08 19:34:32</t>
+  </si>
+  <si>
+    <t>2019-10-08 19:47:40</t>
   </si>
   <si>
     <t>2019-10-08 20:57:02</t>
@@ -5924,11 +5930,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X1031"/>
+  <dimension ref="A1:X1046"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13176,7 +13182,7 @@
         <v>1055</v>
       </c>
       <c r="G340" s="3">
-        <v>6000</v>
+        <v>60000</v>
       </c>
       <c r="H340" s="3"/>
       <c r="I340" s="3" t="s">
@@ -14703,11 +14709,21 @@
       </c>
       <c r="D407" s="3"/>
       <c r="E407" s="3"/>
-      <c r="F407" s="3"/>
-      <c r="G407" s="3"/>
-      <c r="H407" s="3"/>
-      <c r="I407" s="3"/>
-      <c r="J407" s="3"/>
+      <c r="F407" s="3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G407" s="3">
+        <v>0</v>
+      </c>
+      <c r="H407" s="3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="I407" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="J407" s="3" t="s">
+        <v>1271</v>
+      </c>
       <c r="X407" s="3"/>
     </row>
     <row r="408" spans="1:24" x14ac:dyDescent="0.25">
@@ -14732,10 +14748,10 @@
         <v>1062</v>
       </c>
       <c r="I408" s="3" t="s">
-        <v>1270</v>
+        <v>1272</v>
       </c>
       <c r="J408" s="3" t="s">
-        <v>1271</v>
+        <v>1273</v>
       </c>
       <c r="X408" s="3"/>
     </row>
@@ -14761,10 +14777,10 @@
         <v>1062</v>
       </c>
       <c r="I409" s="3" t="s">
-        <v>1272</v>
+        <v>1274</v>
       </c>
       <c r="J409" s="3" t="s">
-        <v>1273</v>
+        <v>1275</v>
       </c>
       <c r="X409" s="3"/>
     </row>
@@ -14790,10 +14806,10 @@
         <v>1062</v>
       </c>
       <c r="I410" s="3" t="s">
-        <v>1274</v>
+        <v>1276</v>
       </c>
       <c r="J410" s="3" t="s">
-        <v>1275</v>
+        <v>1277</v>
       </c>
       <c r="X410" s="3"/>
     </row>
@@ -14819,10 +14835,10 @@
         <v>1062</v>
       </c>
       <c r="I411" s="3" t="s">
-        <v>1276</v>
+        <v>1278</v>
       </c>
       <c r="J411" s="3" t="s">
-        <v>1277</v>
+        <v>1279</v>
       </c>
       <c r="X411" s="3"/>
     </row>
@@ -14848,10 +14864,10 @@
         <v>1062</v>
       </c>
       <c r="I412" s="3" t="s">
-        <v>1278</v>
+        <v>1280</v>
       </c>
       <c r="J412" s="3" t="s">
-        <v>1279</v>
+        <v>1281</v>
       </c>
       <c r="X412" s="3"/>
     </row>
@@ -14877,10 +14893,10 @@
         <v>1062</v>
       </c>
       <c r="I413" s="3" t="s">
-        <v>1280</v>
+        <v>1282</v>
       </c>
       <c r="J413" s="3" t="s">
-        <v>1281</v>
+        <v>1283</v>
       </c>
       <c r="X413" s="3"/>
     </row>
@@ -14906,10 +14922,10 @@
         <v>1062</v>
       </c>
       <c r="I414" s="3" t="s">
-        <v>1282</v>
+        <v>1284</v>
       </c>
       <c r="J414" s="3" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="X414" s="3"/>
     </row>
@@ -14935,10 +14951,10 @@
         <v>1062</v>
       </c>
       <c r="I415" s="3" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="J415" s="3" t="s">
-        <v>1285</v>
+        <v>1287</v>
       </c>
       <c r="X415" s="3"/>
     </row>
@@ -15173,10 +15189,10 @@
         <v>1062</v>
       </c>
       <c r="I427" s="3" t="s">
-        <v>1286</v>
+        <v>1288</v>
       </c>
       <c r="J427" s="3" t="s">
-        <v>1287</v>
+        <v>1289</v>
       </c>
       <c r="X427" s="3"/>
     </row>
@@ -15202,10 +15218,10 @@
         <v>1062</v>
       </c>
       <c r="I428" s="3" t="s">
-        <v>1288</v>
+        <v>1290</v>
       </c>
       <c r="J428" s="3" t="s">
-        <v>1289</v>
+        <v>1291</v>
       </c>
       <c r="X428" s="3"/>
     </row>
@@ -15231,10 +15247,10 @@
         <v>1062</v>
       </c>
       <c r="I429" s="3" t="s">
-        <v>1290</v>
+        <v>1292</v>
       </c>
       <c r="J429" s="3" t="s">
-        <v>1291</v>
+        <v>1293</v>
       </c>
       <c r="X429" s="3"/>
     </row>
@@ -15260,10 +15276,10 @@
         <v>1062</v>
       </c>
       <c r="I430" s="3" t="s">
-        <v>1292</v>
+        <v>1294</v>
       </c>
       <c r="J430" s="3" t="s">
-        <v>1293</v>
+        <v>1295</v>
       </c>
       <c r="X430" s="3"/>
     </row>
@@ -15289,10 +15305,10 @@
         <v>1062</v>
       </c>
       <c r="I431" s="3" t="s">
-        <v>1294</v>
+        <v>1296</v>
       </c>
       <c r="J431" s="3" t="s">
-        <v>1295</v>
+        <v>1297</v>
       </c>
       <c r="X431" s="3"/>
     </row>
@@ -15318,10 +15334,10 @@
         <v>1062</v>
       </c>
       <c r="I432" s="3" t="s">
-        <v>1296</v>
+        <v>1298</v>
       </c>
       <c r="J432" s="3" t="s">
-        <v>1297</v>
+        <v>1299</v>
       </c>
       <c r="X432" s="3"/>
     </row>
@@ -15347,10 +15363,10 @@
         <v>1062</v>
       </c>
       <c r="I433" s="3" t="s">
-        <v>1298</v>
+        <v>1300</v>
       </c>
       <c r="J433" s="3" t="s">
-        <v>1299</v>
+        <v>1301</v>
       </c>
       <c r="X433" s="3"/>
     </row>
@@ -15376,10 +15392,10 @@
         <v>1062</v>
       </c>
       <c r="I434" s="3" t="s">
-        <v>1300</v>
+        <v>1302</v>
       </c>
       <c r="J434" s="3" t="s">
-        <v>1301</v>
+        <v>1303</v>
       </c>
       <c r="X434" s="3"/>
     </row>
@@ -15405,10 +15421,10 @@
         <v>1062</v>
       </c>
       <c r="I435" s="3" t="s">
-        <v>1302</v>
+        <v>1304</v>
       </c>
       <c r="J435" s="3" t="s">
-        <v>1303</v>
+        <v>1305</v>
       </c>
       <c r="X435" s="3"/>
     </row>
@@ -15434,10 +15450,10 @@
         <v>1062</v>
       </c>
       <c r="I436" s="3" t="s">
-        <v>1304</v>
+        <v>1306</v>
       </c>
       <c r="J436" s="3" t="s">
-        <v>1305</v>
+        <v>1307</v>
       </c>
       <c r="X436" s="3"/>
     </row>
@@ -15463,10 +15479,10 @@
         <v>1062</v>
       </c>
       <c r="I437" s="3" t="s">
-        <v>1306</v>
+        <v>1308</v>
       </c>
       <c r="J437" s="3" t="s">
-        <v>1307</v>
+        <v>1309</v>
       </c>
       <c r="X437" s="3"/>
     </row>
@@ -15492,10 +15508,10 @@
         <v>1062</v>
       </c>
       <c r="I438" s="3" t="s">
-        <v>1308</v>
+        <v>1310</v>
       </c>
       <c r="J438" s="3" t="s">
-        <v>1309</v>
+        <v>1311</v>
       </c>
       <c r="X438" s="3"/>
     </row>
@@ -15521,10 +15537,10 @@
         <v>1062</v>
       </c>
       <c r="I439" s="3" t="s">
-        <v>1310</v>
+        <v>1312</v>
       </c>
       <c r="J439" s="3" t="s">
-        <v>1311</v>
+        <v>1313</v>
       </c>
       <c r="X439" s="3"/>
     </row>
@@ -15550,10 +15566,10 @@
         <v>1062</v>
       </c>
       <c r="I440" s="3" t="s">
-        <v>1312</v>
+        <v>1314</v>
       </c>
       <c r="J440" s="3" t="s">
-        <v>1313</v>
+        <v>1315</v>
       </c>
       <c r="X440" s="3"/>
     </row>
@@ -15579,10 +15595,10 @@
         <v>1062</v>
       </c>
       <c r="I441" s="3" t="s">
-        <v>1314</v>
+        <v>1316</v>
       </c>
       <c r="J441" s="3" t="s">
-        <v>1315</v>
+        <v>1317</v>
       </c>
       <c r="X441" s="3"/>
     </row>
@@ -15608,10 +15624,10 @@
         <v>1062</v>
       </c>
       <c r="I442" s="3" t="s">
-        <v>1316</v>
+        <v>1318</v>
       </c>
       <c r="J442" s="3" t="s">
-        <v>1317</v>
+        <v>1319</v>
       </c>
       <c r="X442" s="3"/>
     </row>
@@ -15637,10 +15653,10 @@
         <v>1062</v>
       </c>
       <c r="I443" s="3" t="s">
-        <v>1318</v>
+        <v>1320</v>
       </c>
       <c r="J443" s="3" t="s">
-        <v>1319</v>
+        <v>1321</v>
       </c>
       <c r="X443" s="3"/>
     </row>
@@ -15666,10 +15682,10 @@
         <v>1062</v>
       </c>
       <c r="I444" s="3" t="s">
-        <v>1320</v>
+        <v>1322</v>
       </c>
       <c r="J444" s="3" t="s">
-        <v>1321</v>
+        <v>1323</v>
       </c>
       <c r="X444" s="3"/>
     </row>
@@ -15695,10 +15711,10 @@
         <v>1062</v>
       </c>
       <c r="I445" s="3" t="s">
-        <v>1322</v>
+        <v>1324</v>
       </c>
       <c r="J445" s="3" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
       <c r="X445" s="3"/>
     </row>
@@ -15724,10 +15740,10 @@
         <v>1062</v>
       </c>
       <c r="I446" s="3" t="s">
-        <v>1324</v>
+        <v>1326</v>
       </c>
       <c r="J446" s="3" t="s">
-        <v>1325</v>
+        <v>1327</v>
       </c>
       <c r="X446" s="3"/>
     </row>
@@ -20425,10 +20441,10 @@
       </c>
       <c r="H693" s="3"/>
       <c r="I693" s="3" t="s">
-        <v>1326</v>
+        <v>1328</v>
       </c>
       <c r="J693" s="3" t="s">
-        <v>1326</v>
+        <v>1328</v>
       </c>
       <c r="X693" s="3"/>
     </row>
@@ -20452,10 +20468,10 @@
       </c>
       <c r="H694" s="3"/>
       <c r="I694" s="3" t="s">
-        <v>1327</v>
+        <v>1329</v>
       </c>
       <c r="J694" s="3" t="s">
-        <v>1328</v>
+        <v>1330</v>
       </c>
       <c r="X694" s="3"/>
     </row>
@@ -20954,10 +20970,10 @@
       </c>
       <c r="H720" s="3"/>
       <c r="I720" s="3" t="s">
-        <v>1329</v>
+        <v>1331</v>
       </c>
       <c r="J720" s="3" t="s">
-        <v>1330</v>
+        <v>1332</v>
       </c>
       <c r="X720" s="3"/>
     </row>
@@ -20981,10 +20997,10 @@
       </c>
       <c r="H721" s="3"/>
       <c r="I721" s="3" t="s">
-        <v>1331</v>
+        <v>1333</v>
       </c>
       <c r="J721" s="3" t="s">
-        <v>1332</v>
+        <v>1334</v>
       </c>
       <c r="X721" s="3"/>
     </row>
@@ -21008,10 +21024,10 @@
       </c>
       <c r="H722" s="3"/>
       <c r="I722" s="3" t="s">
-        <v>1333</v>
+        <v>1335</v>
       </c>
       <c r="J722" s="3" t="s">
-        <v>1334</v>
+        <v>1336</v>
       </c>
       <c r="X722" s="3"/>
     </row>
@@ -21035,10 +21051,10 @@
       </c>
       <c r="H723" s="3"/>
       <c r="I723" s="3" t="s">
-        <v>1335</v>
+        <v>1337</v>
       </c>
       <c r="J723" s="3" t="s">
-        <v>1336</v>
+        <v>1338</v>
       </c>
       <c r="X723" s="3"/>
     </row>
@@ -21062,10 +21078,10 @@
       </c>
       <c r="H724" s="3"/>
       <c r="I724" s="3" t="s">
-        <v>1337</v>
+        <v>1339</v>
       </c>
       <c r="J724" s="3" t="s">
-        <v>1338</v>
+        <v>1340</v>
       </c>
       <c r="X724" s="3"/>
     </row>
@@ -21127,10 +21143,10 @@
       </c>
       <c r="H727" s="3"/>
       <c r="I727" s="3" t="s">
-        <v>1339</v>
+        <v>1341</v>
       </c>
       <c r="J727" s="3" t="s">
-        <v>1340</v>
+        <v>1342</v>
       </c>
       <c r="X727" s="3"/>
     </row>
@@ -21151,7 +21167,7 @@
       <c r="H728" s="3"/>
       <c r="I728" s="3"/>
       <c r="J728" s="3" t="s">
-        <v>1341</v>
+        <v>1343</v>
       </c>
       <c r="X728" s="3"/>
     </row>
@@ -21172,7 +21188,7 @@
       <c r="H729" s="3"/>
       <c r="I729" s="3"/>
       <c r="J729" s="3" t="s">
-        <v>1342</v>
+        <v>1344</v>
       </c>
       <c r="X729" s="3"/>
     </row>
@@ -21193,7 +21209,7 @@
       <c r="H730" s="3"/>
       <c r="I730" s="3"/>
       <c r="J730" s="3" t="s">
-        <v>1343</v>
+        <v>1345</v>
       </c>
       <c r="X730" s="3"/>
     </row>
@@ -21214,7 +21230,7 @@
       <c r="H731" s="3"/>
       <c r="I731" s="3"/>
       <c r="J731" s="3" t="s">
-        <v>1344</v>
+        <v>1346</v>
       </c>
       <c r="X731" s="3"/>
     </row>
@@ -21235,7 +21251,7 @@
       <c r="H732" s="3"/>
       <c r="I732" s="3"/>
       <c r="J732" s="3" t="s">
-        <v>1345</v>
+        <v>1347</v>
       </c>
       <c r="X732" s="3"/>
     </row>
@@ -21256,7 +21272,7 @@
       <c r="H733" s="3"/>
       <c r="I733" s="3"/>
       <c r="J733" s="3" t="s">
-        <v>1346</v>
+        <v>1348</v>
       </c>
       <c r="X733" s="3"/>
     </row>
@@ -21277,7 +21293,7 @@
       <c r="H734" s="3"/>
       <c r="I734" s="3"/>
       <c r="J734" s="3" t="s">
-        <v>1347</v>
+        <v>1349</v>
       </c>
       <c r="X734" s="3"/>
     </row>
@@ -21298,7 +21314,7 @@
       <c r="H735" s="3"/>
       <c r="I735" s="3"/>
       <c r="J735" s="3" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="X735" s="3"/>
     </row>
@@ -21322,10 +21338,10 @@
       </c>
       <c r="H736" s="3"/>
       <c r="I736" s="3" t="s">
-        <v>1349</v>
+        <v>1351</v>
       </c>
       <c r="J736" s="3" t="s">
-        <v>1350</v>
+        <v>1352</v>
       </c>
       <c r="X736" s="3"/>
     </row>
@@ -21346,7 +21362,7 @@
       <c r="H737" s="3"/>
       <c r="I737" s="3"/>
       <c r="J737" s="3" t="s">
-        <v>1351</v>
+        <v>1353</v>
       </c>
       <c r="X737" s="3"/>
     </row>
@@ -21367,7 +21383,7 @@
       <c r="H738" s="3"/>
       <c r="I738" s="3"/>
       <c r="J738" s="3" t="s">
-        <v>1352</v>
+        <v>1354</v>
       </c>
       <c r="X738" s="3"/>
     </row>
@@ -21388,7 +21404,7 @@
       <c r="H739" s="3"/>
       <c r="I739" s="3"/>
       <c r="J739" s="3" t="s">
-        <v>1353</v>
+        <v>1355</v>
       </c>
       <c r="X739" s="3"/>
     </row>
@@ -21409,7 +21425,7 @@
       <c r="H740" s="3"/>
       <c r="I740" s="3"/>
       <c r="J740" s="3" t="s">
-        <v>1354</v>
+        <v>1356</v>
       </c>
       <c r="X740" s="3"/>
     </row>
@@ -21430,7 +21446,7 @@
       <c r="H741" s="3"/>
       <c r="I741" s="3"/>
       <c r="J741" s="3" t="s">
-        <v>1355</v>
+        <v>1357</v>
       </c>
       <c r="X741" s="3"/>
     </row>
@@ -21451,7 +21467,7 @@
       <c r="H742" s="3"/>
       <c r="I742" s="3"/>
       <c r="J742" s="3" t="s">
-        <v>1356</v>
+        <v>1358</v>
       </c>
       <c r="X742" s="3"/>
     </row>
@@ -21472,7 +21488,7 @@
       <c r="H743" s="3"/>
       <c r="I743" s="3"/>
       <c r="J743" s="3" t="s">
-        <v>1357</v>
+        <v>1359</v>
       </c>
       <c r="X743" s="3"/>
     </row>
@@ -21496,10 +21512,10 @@
       </c>
       <c r="H744" s="3"/>
       <c r="I744" s="3" t="s">
-        <v>1358</v>
+        <v>1360</v>
       </c>
       <c r="J744" s="3" t="s">
-        <v>1359</v>
+        <v>1361</v>
       </c>
       <c r="X744" s="3"/>
     </row>
@@ -21523,10 +21539,10 @@
       </c>
       <c r="H745" s="3"/>
       <c r="I745" s="3" t="s">
-        <v>1360</v>
+        <v>1362</v>
       </c>
       <c r="J745" s="3" t="s">
-        <v>1361</v>
+        <v>1363</v>
       </c>
       <c r="X745" s="3"/>
     </row>
@@ -21550,10 +21566,10 @@
       </c>
       <c r="H746" s="3"/>
       <c r="I746" s="3" t="s">
-        <v>1362</v>
+        <v>1364</v>
       </c>
       <c r="J746" s="3" t="s">
-        <v>1363</v>
+        <v>1365</v>
       </c>
       <c r="X746" s="3"/>
     </row>
@@ -21577,10 +21593,10 @@
       </c>
       <c r="H747" s="3"/>
       <c r="I747" s="3" t="s">
-        <v>1364</v>
+        <v>1366</v>
       </c>
       <c r="J747" s="3" t="s">
-        <v>1365</v>
+        <v>1367</v>
       </c>
       <c r="X747" s="3"/>
     </row>
@@ -21604,10 +21620,10 @@
       </c>
       <c r="H748" s="3"/>
       <c r="I748" s="3" t="s">
-        <v>1366</v>
+        <v>1368</v>
       </c>
       <c r="J748" s="3" t="s">
-        <v>1367</v>
+        <v>1369</v>
       </c>
       <c r="X748" s="3"/>
     </row>
@@ -21631,10 +21647,10 @@
       </c>
       <c r="H749" s="3"/>
       <c r="I749" s="3" t="s">
-        <v>1368</v>
+        <v>1370</v>
       </c>
       <c r="J749" s="3" t="s">
-        <v>1369</v>
+        <v>1371</v>
       </c>
       <c r="X749" s="3"/>
     </row>
@@ -21658,10 +21674,10 @@
       </c>
       <c r="H750" s="3"/>
       <c r="I750" s="3" t="s">
-        <v>1370</v>
+        <v>1372</v>
       </c>
       <c r="J750" s="3" t="s">
-        <v>1371</v>
+        <v>1373</v>
       </c>
       <c r="X750" s="3"/>
     </row>
@@ -21685,10 +21701,10 @@
       </c>
       <c r="H751" s="3"/>
       <c r="I751" s="3" t="s">
-        <v>1372</v>
+        <v>1374</v>
       </c>
       <c r="J751" s="3" t="s">
-        <v>1373</v>
+        <v>1375</v>
       </c>
       <c r="X751" s="3"/>
     </row>
@@ -21712,10 +21728,10 @@
       </c>
       <c r="H752" s="3"/>
       <c r="I752" s="3" t="s">
-        <v>1374</v>
+        <v>1376</v>
       </c>
       <c r="J752" s="3" t="s">
-        <v>1375</v>
+        <v>1377</v>
       </c>
       <c r="X752" s="3"/>
     </row>
@@ -21739,10 +21755,10 @@
       </c>
       <c r="H753" s="3"/>
       <c r="I753" s="3" t="s">
-        <v>1376</v>
+        <v>1378</v>
       </c>
       <c r="J753" s="3" t="s">
-        <v>1377</v>
+        <v>1379</v>
       </c>
       <c r="X753" s="3"/>
     </row>
@@ -21766,10 +21782,10 @@
       </c>
       <c r="H754" s="3"/>
       <c r="I754" s="3" t="s">
-        <v>1378</v>
+        <v>1380</v>
       </c>
       <c r="J754" s="3" t="s">
-        <v>1379</v>
+        <v>1381</v>
       </c>
       <c r="X754" s="3"/>
     </row>
@@ -21793,10 +21809,10 @@
       </c>
       <c r="H755" s="3"/>
       <c r="I755" s="3" t="s">
-        <v>1380</v>
+        <v>1382</v>
       </c>
       <c r="J755" s="3" t="s">
-        <v>1381</v>
+        <v>1383</v>
       </c>
       <c r="X755" s="3"/>
     </row>
@@ -21817,7 +21833,7 @@
       <c r="H756" s="3"/>
       <c r="I756" s="3"/>
       <c r="J756" s="3" t="s">
-        <v>1382</v>
+        <v>1384</v>
       </c>
       <c r="X756" s="3"/>
     </row>
@@ -21841,10 +21857,10 @@
       </c>
       <c r="H757" s="3"/>
       <c r="I757" s="3" t="s">
-        <v>1383</v>
+        <v>1385</v>
       </c>
       <c r="J757" s="3" t="s">
-        <v>1384</v>
+        <v>1386</v>
       </c>
       <c r="X757" s="3"/>
     </row>
@@ -21868,10 +21884,10 @@
       </c>
       <c r="H758" s="3"/>
       <c r="I758" s="3" t="s">
-        <v>1385</v>
+        <v>1387</v>
       </c>
       <c r="J758" s="3" t="s">
-        <v>1386</v>
+        <v>1388</v>
       </c>
       <c r="X758" s="3"/>
     </row>
@@ -21895,10 +21911,10 @@
       </c>
       <c r="H759" s="3"/>
       <c r="I759" s="3" t="s">
-        <v>1387</v>
+        <v>1389</v>
       </c>
       <c r="J759" s="3" t="s">
-        <v>1388</v>
+        <v>1390</v>
       </c>
       <c r="X759" s="3"/>
     </row>
@@ -21922,10 +21938,10 @@
       </c>
       <c r="H760" s="3"/>
       <c r="I760" s="3" t="s">
-        <v>1389</v>
+        <v>1391</v>
       </c>
       <c r="J760" s="3" t="s">
-        <v>1390</v>
+        <v>1392</v>
       </c>
       <c r="X760" s="3"/>
     </row>
@@ -21949,10 +21965,10 @@
       </c>
       <c r="H761" s="3"/>
       <c r="I761" s="3" t="s">
-        <v>1391</v>
+        <v>1393</v>
       </c>
       <c r="J761" s="3" t="s">
-        <v>1392</v>
+        <v>1394</v>
       </c>
       <c r="X761" s="3"/>
     </row>
@@ -21976,10 +21992,10 @@
       </c>
       <c r="H762" s="3"/>
       <c r="I762" s="3" t="s">
-        <v>1393</v>
+        <v>1395</v>
       </c>
       <c r="J762" s="3" t="s">
-        <v>1394</v>
+        <v>1396</v>
       </c>
       <c r="X762" s="3"/>
     </row>
@@ -22003,10 +22019,10 @@
       </c>
       <c r="H763" s="3"/>
       <c r="I763" s="3" t="s">
-        <v>1395</v>
+        <v>1397</v>
       </c>
       <c r="J763" s="3" t="s">
-        <v>1396</v>
+        <v>1398</v>
       </c>
       <c r="X763" s="3"/>
     </row>
@@ -22030,10 +22046,10 @@
       </c>
       <c r="H764" s="3"/>
       <c r="I764" s="3" t="s">
-        <v>1397</v>
+        <v>1399</v>
       </c>
       <c r="J764" s="3" t="s">
-        <v>1398</v>
+        <v>1400</v>
       </c>
       <c r="X764" s="3"/>
     </row>
@@ -22057,10 +22073,10 @@
       </c>
       <c r="H765" s="3"/>
       <c r="I765" s="3" t="s">
-        <v>1399</v>
+        <v>1401</v>
       </c>
       <c r="J765" s="3" t="s">
-        <v>1400</v>
+        <v>1402</v>
       </c>
       <c r="X765" s="3"/>
     </row>
@@ -22084,10 +22100,10 @@
       </c>
       <c r="H766" s="3"/>
       <c r="I766" s="3" t="s">
-        <v>1401</v>
+        <v>1403</v>
       </c>
       <c r="J766" s="3" t="s">
-        <v>1402</v>
+        <v>1404</v>
       </c>
       <c r="X766" s="3"/>
     </row>
@@ -22111,10 +22127,10 @@
       </c>
       <c r="H767" s="3"/>
       <c r="I767" s="3" t="s">
-        <v>1403</v>
+        <v>1405</v>
       </c>
       <c r="J767" s="3" t="s">
-        <v>1404</v>
+        <v>1406</v>
       </c>
       <c r="X767" s="3"/>
     </row>
@@ -22138,10 +22154,10 @@
       </c>
       <c r="H768" s="3"/>
       <c r="I768" s="3" t="s">
-        <v>1405</v>
+        <v>1407</v>
       </c>
       <c r="J768" s="3" t="s">
-        <v>1406</v>
+        <v>1408</v>
       </c>
       <c r="X768" s="3"/>
     </row>
@@ -22165,10 +22181,10 @@
       </c>
       <c r="H769" s="3"/>
       <c r="I769" s="3" t="s">
-        <v>1407</v>
+        <v>1409</v>
       </c>
       <c r="J769" s="3" t="s">
-        <v>1408</v>
+        <v>1410</v>
       </c>
       <c r="X769" s="3"/>
     </row>
@@ -22192,10 +22208,10 @@
       </c>
       <c r="H770" s="3"/>
       <c r="I770" s="3" t="s">
-        <v>1409</v>
+        <v>1411</v>
       </c>
       <c r="J770" s="3" t="s">
-        <v>1410</v>
+        <v>1412</v>
       </c>
       <c r="X770" s="3"/>
     </row>
@@ -22219,10 +22235,10 @@
       </c>
       <c r="H771" s="3"/>
       <c r="I771" s="3" t="s">
-        <v>1411</v>
+        <v>1413</v>
       </c>
       <c r="J771" s="3" t="s">
-        <v>1412</v>
+        <v>1414</v>
       </c>
       <c r="X771" s="3"/>
     </row>
@@ -22246,10 +22262,10 @@
       </c>
       <c r="H772" s="3"/>
       <c r="I772" s="3" t="s">
-        <v>1413</v>
+        <v>1415</v>
       </c>
       <c r="J772" s="3" t="s">
-        <v>1414</v>
+        <v>1416</v>
       </c>
       <c r="X772" s="3"/>
     </row>
@@ -22273,10 +22289,10 @@
       </c>
       <c r="H773" s="3"/>
       <c r="I773" s="3" t="s">
-        <v>1415</v>
+        <v>1417</v>
       </c>
       <c r="J773" s="3" t="s">
-        <v>1416</v>
+        <v>1418</v>
       </c>
       <c r="X773" s="3"/>
     </row>
@@ -22300,10 +22316,10 @@
       </c>
       <c r="H774" s="3"/>
       <c r="I774" s="3" t="s">
-        <v>1417</v>
+        <v>1419</v>
       </c>
       <c r="J774" s="3" t="s">
-        <v>1418</v>
+        <v>1420</v>
       </c>
       <c r="X774" s="3"/>
     </row>
@@ -22327,10 +22343,10 @@
       </c>
       <c r="H775" s="3"/>
       <c r="I775" s="3" t="s">
-        <v>1419</v>
+        <v>1421</v>
       </c>
       <c r="J775" s="3" t="s">
-        <v>1420</v>
+        <v>1422</v>
       </c>
       <c r="X775" s="3"/>
     </row>
@@ -22354,10 +22370,10 @@
       </c>
       <c r="H776" s="3"/>
       <c r="I776" s="3" t="s">
-        <v>1421</v>
+        <v>1423</v>
       </c>
       <c r="J776" s="3" t="s">
-        <v>1422</v>
+        <v>1424</v>
       </c>
       <c r="X776" s="3"/>
     </row>
@@ -22381,10 +22397,10 @@
       </c>
       <c r="H777" s="3"/>
       <c r="I777" s="3" t="s">
-        <v>1423</v>
+        <v>1425</v>
       </c>
       <c r="J777" s="3" t="s">
-        <v>1424</v>
+        <v>1426</v>
       </c>
       <c r="X777" s="3"/>
     </row>
@@ -22408,10 +22424,10 @@
       </c>
       <c r="H778" s="3"/>
       <c r="I778" s="3" t="s">
-        <v>1425</v>
+        <v>1427</v>
       </c>
       <c r="J778" s="3" t="s">
-        <v>1426</v>
+        <v>1428</v>
       </c>
       <c r="X778" s="3"/>
     </row>
@@ -22435,10 +22451,10 @@
       </c>
       <c r="H779" s="3"/>
       <c r="I779" s="3" t="s">
-        <v>1427</v>
+        <v>1429</v>
       </c>
       <c r="J779" s="3" t="s">
-        <v>1428</v>
+        <v>1430</v>
       </c>
       <c r="X779" s="3"/>
     </row>
@@ -22462,10 +22478,10 @@
       </c>
       <c r="H780" s="3"/>
       <c r="I780" s="3" t="s">
-        <v>1429</v>
+        <v>1431</v>
       </c>
       <c r="J780" s="3" t="s">
-        <v>1430</v>
+        <v>1432</v>
       </c>
       <c r="X780" s="3"/>
     </row>
@@ -22489,10 +22505,10 @@
       </c>
       <c r="H781" s="3"/>
       <c r="I781" s="3" t="s">
-        <v>1431</v>
+        <v>1433</v>
       </c>
       <c r="J781" s="3" t="s">
-        <v>1432</v>
+        <v>1434</v>
       </c>
       <c r="X781" s="3"/>
     </row>
@@ -22516,10 +22532,10 @@
       </c>
       <c r="H782" s="3"/>
       <c r="I782" s="3" t="s">
-        <v>1433</v>
+        <v>1435</v>
       </c>
       <c r="J782" s="3" t="s">
-        <v>1434</v>
+        <v>1436</v>
       </c>
       <c r="X782" s="3"/>
     </row>
@@ -22543,10 +22559,10 @@
       </c>
       <c r="H783" s="3"/>
       <c r="I783" s="3" t="s">
-        <v>1435</v>
+        <v>1437</v>
       </c>
       <c r="J783" s="3" t="s">
-        <v>1436</v>
+        <v>1438</v>
       </c>
       <c r="X783" s="3"/>
     </row>
@@ -22570,10 +22586,10 @@
       </c>
       <c r="H784" s="3"/>
       <c r="I784" s="3" t="s">
-        <v>1437</v>
+        <v>1439</v>
       </c>
       <c r="J784" s="3" t="s">
-        <v>1438</v>
+        <v>1440</v>
       </c>
       <c r="X784" s="3"/>
     </row>
@@ -22597,10 +22613,10 @@
       </c>
       <c r="H785" s="3"/>
       <c r="I785" s="3" t="s">
-        <v>1439</v>
+        <v>1441</v>
       </c>
       <c r="J785" s="3" t="s">
-        <v>1440</v>
+        <v>1442</v>
       </c>
       <c r="X785" s="3"/>
     </row>
@@ -22624,10 +22640,10 @@
       </c>
       <c r="H786" s="3"/>
       <c r="I786" s="3" t="s">
-        <v>1441</v>
+        <v>1443</v>
       </c>
       <c r="J786" s="3" t="s">
-        <v>1442</v>
+        <v>1444</v>
       </c>
       <c r="X786" s="3"/>
     </row>
@@ -22651,10 +22667,10 @@
       </c>
       <c r="H787" s="3"/>
       <c r="I787" s="3" t="s">
-        <v>1443</v>
+        <v>1445</v>
       </c>
       <c r="J787" s="3" t="s">
-        <v>1444</v>
+        <v>1446</v>
       </c>
       <c r="X787" s="3"/>
     </row>
@@ -22678,10 +22694,10 @@
       </c>
       <c r="H788" s="3"/>
       <c r="I788" s="3" t="s">
-        <v>1445</v>
+        <v>1447</v>
       </c>
       <c r="J788" s="3" t="s">
-        <v>1446</v>
+        <v>1448</v>
       </c>
       <c r="X788" s="3"/>
     </row>
@@ -22705,10 +22721,10 @@
       </c>
       <c r="H789" s="3"/>
       <c r="I789" s="3" t="s">
-        <v>1447</v>
+        <v>1449</v>
       </c>
       <c r="J789" s="3" t="s">
-        <v>1448</v>
+        <v>1450</v>
       </c>
       <c r="X789" s="3"/>
     </row>
@@ -22732,10 +22748,10 @@
       </c>
       <c r="H790" s="3"/>
       <c r="I790" s="3" t="s">
-        <v>1449</v>
+        <v>1451</v>
       </c>
       <c r="J790" s="3" t="s">
-        <v>1450</v>
+        <v>1452</v>
       </c>
       <c r="X790" s="3"/>
     </row>
@@ -22759,10 +22775,10 @@
       </c>
       <c r="H791" s="3"/>
       <c r="I791" s="3" t="s">
-        <v>1451</v>
+        <v>1453</v>
       </c>
       <c r="J791" s="3" t="s">
-        <v>1452</v>
+        <v>1454</v>
       </c>
       <c r="X791" s="3"/>
     </row>
@@ -22786,10 +22802,10 @@
       </c>
       <c r="H792" s="3"/>
       <c r="I792" s="3" t="s">
-        <v>1453</v>
+        <v>1455</v>
       </c>
       <c r="J792" s="3" t="s">
-        <v>1454</v>
+        <v>1456</v>
       </c>
       <c r="X792" s="3"/>
     </row>
@@ -22813,10 +22829,10 @@
       </c>
       <c r="H793" s="3"/>
       <c r="I793" s="3" t="s">
-        <v>1455</v>
+        <v>1457</v>
       </c>
       <c r="J793" s="3" t="s">
-        <v>1456</v>
+        <v>1458</v>
       </c>
       <c r="X793" s="3"/>
     </row>
@@ -22840,10 +22856,10 @@
       </c>
       <c r="H794" s="3"/>
       <c r="I794" s="3" t="s">
-        <v>1457</v>
+        <v>1459</v>
       </c>
       <c r="J794" s="3" t="s">
-        <v>1458</v>
+        <v>1460</v>
       </c>
       <c r="X794" s="3"/>
     </row>
@@ -22867,10 +22883,10 @@
       </c>
       <c r="H795" s="3"/>
       <c r="I795" s="3" t="s">
-        <v>1459</v>
+        <v>1461</v>
       </c>
       <c r="J795" s="3" t="s">
-        <v>1460</v>
+        <v>1462</v>
       </c>
       <c r="X795" s="3"/>
     </row>
@@ -22894,10 +22910,10 @@
       </c>
       <c r="H796" s="3"/>
       <c r="I796" s="3" t="s">
-        <v>1461</v>
+        <v>1463</v>
       </c>
       <c r="J796" s="3" t="s">
-        <v>1462</v>
+        <v>1464</v>
       </c>
       <c r="X796" s="3"/>
     </row>
@@ -22921,10 +22937,10 @@
       </c>
       <c r="H797" s="3"/>
       <c r="I797" s="3" t="s">
-        <v>1463</v>
+        <v>1465</v>
       </c>
       <c r="J797" s="3" t="s">
-        <v>1464</v>
+        <v>1466</v>
       </c>
       <c r="X797" s="3"/>
     </row>
@@ -22948,10 +22964,10 @@
       </c>
       <c r="H798" s="3"/>
       <c r="I798" s="3" t="s">
-        <v>1465</v>
+        <v>1467</v>
       </c>
       <c r="J798" s="3" t="s">
-        <v>1466</v>
+        <v>1468</v>
       </c>
       <c r="X798" s="3"/>
     </row>
@@ -22975,10 +22991,10 @@
       </c>
       <c r="H799" s="3"/>
       <c r="I799" s="3" t="s">
-        <v>1467</v>
+        <v>1469</v>
       </c>
       <c r="J799" s="3" t="s">
-        <v>1468</v>
+        <v>1470</v>
       </c>
       <c r="X799" s="3"/>
     </row>
@@ -23002,10 +23018,10 @@
       </c>
       <c r="H800" s="3"/>
       <c r="I800" s="3" t="s">
-        <v>1469</v>
+        <v>1471</v>
       </c>
       <c r="J800" s="3" t="s">
-        <v>1470</v>
+        <v>1472</v>
       </c>
       <c r="X800" s="3"/>
     </row>
@@ -23029,10 +23045,10 @@
       </c>
       <c r="H801" s="3"/>
       <c r="I801" s="3" t="s">
-        <v>1471</v>
+        <v>1473</v>
       </c>
       <c r="J801" s="3" t="s">
-        <v>1472</v>
+        <v>1474</v>
       </c>
       <c r="X801" s="3"/>
     </row>
@@ -23056,10 +23072,10 @@
       </c>
       <c r="H802" s="3"/>
       <c r="I802" s="3" t="s">
-        <v>1473</v>
+        <v>1475</v>
       </c>
       <c r="J802" s="3" t="s">
-        <v>1474</v>
+        <v>1476</v>
       </c>
       <c r="X802" s="3"/>
     </row>
@@ -23083,10 +23099,10 @@
       </c>
       <c r="H803" s="3"/>
       <c r="I803" s="3" t="s">
-        <v>1475</v>
+        <v>1477</v>
       </c>
       <c r="J803" s="3" t="s">
-        <v>1476</v>
+        <v>1478</v>
       </c>
       <c r="X803" s="3"/>
     </row>
@@ -23110,10 +23126,10 @@
       </c>
       <c r="H804" s="3"/>
       <c r="I804" s="3" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
       <c r="J804" s="3" t="s">
-        <v>1478</v>
+        <v>1480</v>
       </c>
       <c r="X804" s="3"/>
     </row>
@@ -23137,10 +23153,10 @@
       </c>
       <c r="H805" s="3"/>
       <c r="I805" s="3" t="s">
-        <v>1479</v>
+        <v>1481</v>
       </c>
       <c r="J805" s="3" t="s">
-        <v>1480</v>
+        <v>1482</v>
       </c>
       <c r="X805" s="3"/>
     </row>
@@ -23164,10 +23180,10 @@
       </c>
       <c r="H806" s="3"/>
       <c r="I806" s="3" t="s">
-        <v>1481</v>
+        <v>1483</v>
       </c>
       <c r="J806" s="3" t="s">
-        <v>1482</v>
+        <v>1484</v>
       </c>
       <c r="X806" s="3"/>
     </row>
@@ -23191,10 +23207,10 @@
       </c>
       <c r="H807" s="3"/>
       <c r="I807" s="3" t="s">
-        <v>1483</v>
+        <v>1485</v>
       </c>
       <c r="J807" s="3" t="s">
-        <v>1484</v>
+        <v>1486</v>
       </c>
       <c r="X807" s="3"/>
     </row>
@@ -23218,10 +23234,10 @@
       </c>
       <c r="H808" s="3"/>
       <c r="I808" s="3" t="s">
-        <v>1485</v>
+        <v>1487</v>
       </c>
       <c r="J808" s="3" t="s">
-        <v>1486</v>
+        <v>1488</v>
       </c>
       <c r="X808" s="3"/>
     </row>
@@ -23245,10 +23261,10 @@
       </c>
       <c r="H809" s="3"/>
       <c r="I809" s="3" t="s">
-        <v>1487</v>
+        <v>1489</v>
       </c>
       <c r="J809" s="3" t="s">
-        <v>1488</v>
+        <v>1490</v>
       </c>
       <c r="X809" s="3"/>
     </row>
@@ -23272,10 +23288,10 @@
       </c>
       <c r="H810" s="3"/>
       <c r="I810" s="3" t="s">
-        <v>1489</v>
+        <v>1491</v>
       </c>
       <c r="J810" s="3" t="s">
-        <v>1490</v>
+        <v>1492</v>
       </c>
       <c r="X810" s="3"/>
     </row>
@@ -23299,10 +23315,10 @@
       </c>
       <c r="H811" s="3"/>
       <c r="I811" s="3" t="s">
-        <v>1491</v>
+        <v>1493</v>
       </c>
       <c r="J811" s="3" t="s">
-        <v>1492</v>
+        <v>1494</v>
       </c>
       <c r="X811" s="3"/>
     </row>
@@ -23326,10 +23342,10 @@
       </c>
       <c r="H812" s="3"/>
       <c r="I812" s="3" t="s">
-        <v>1493</v>
+        <v>1495</v>
       </c>
       <c r="J812" s="3" t="s">
-        <v>1494</v>
+        <v>1496</v>
       </c>
       <c r="X812" s="3"/>
     </row>
@@ -23353,10 +23369,10 @@
       </c>
       <c r="H813" s="3"/>
       <c r="I813" s="3" t="s">
-        <v>1495</v>
+        <v>1497</v>
       </c>
       <c r="J813" s="3" t="s">
-        <v>1496</v>
+        <v>1498</v>
       </c>
       <c r="X813" s="3"/>
     </row>
@@ -23380,10 +23396,10 @@
       </c>
       <c r="H814" s="3"/>
       <c r="I814" s="3" t="s">
-        <v>1497</v>
+        <v>1499</v>
       </c>
       <c r="J814" s="3" t="s">
-        <v>1498</v>
+        <v>1500</v>
       </c>
       <c r="X814" s="3"/>
     </row>
@@ -23407,10 +23423,10 @@
       </c>
       <c r="H815" s="3"/>
       <c r="I815" s="3" t="s">
-        <v>1499</v>
+        <v>1501</v>
       </c>
       <c r="J815" s="3" t="s">
-        <v>1500</v>
+        <v>1502</v>
       </c>
       <c r="X815" s="3"/>
     </row>
@@ -23434,10 +23450,10 @@
       </c>
       <c r="H816" s="3"/>
       <c r="I816" s="3" t="s">
-        <v>1501</v>
+        <v>1503</v>
       </c>
       <c r="J816" s="3" t="s">
-        <v>1502</v>
+        <v>1504</v>
       </c>
       <c r="X816" s="3"/>
     </row>
@@ -23461,10 +23477,10 @@
       </c>
       <c r="H817" s="3"/>
       <c r="I817" s="3" t="s">
-        <v>1503</v>
+        <v>1505</v>
       </c>
       <c r="J817" s="3" t="s">
-        <v>1504</v>
+        <v>1506</v>
       </c>
       <c r="X817" s="3"/>
     </row>
@@ -23488,10 +23504,10 @@
       </c>
       <c r="H818" s="3"/>
       <c r="I818" s="3" t="s">
-        <v>1505</v>
+        <v>1507</v>
       </c>
       <c r="J818" s="3" t="s">
-        <v>1506</v>
+        <v>1508</v>
       </c>
       <c r="X818" s="3"/>
     </row>
@@ -23515,10 +23531,10 @@
       </c>
       <c r="H819" s="3"/>
       <c r="I819" s="3" t="s">
-        <v>1507</v>
+        <v>1509</v>
       </c>
       <c r="J819" s="3" t="s">
-        <v>1508</v>
+        <v>1510</v>
       </c>
       <c r="X819" s="3"/>
     </row>
@@ -23542,10 +23558,10 @@
       </c>
       <c r="H820" s="3"/>
       <c r="I820" s="3" t="s">
-        <v>1509</v>
+        <v>1511</v>
       </c>
       <c r="J820" s="3" t="s">
-        <v>1510</v>
+        <v>1512</v>
       </c>
       <c r="X820" s="3"/>
     </row>
@@ -23569,10 +23585,10 @@
       </c>
       <c r="H821" s="3"/>
       <c r="I821" s="3" t="s">
-        <v>1511</v>
+        <v>1513</v>
       </c>
       <c r="J821" s="3" t="s">
-        <v>1512</v>
+        <v>1514</v>
       </c>
       <c r="X821" s="3"/>
     </row>
@@ -23596,10 +23612,10 @@
       </c>
       <c r="H822" s="3"/>
       <c r="I822" s="3" t="s">
-        <v>1513</v>
+        <v>1515</v>
       </c>
       <c r="J822" s="3" t="s">
-        <v>1514</v>
+        <v>1516</v>
       </c>
       <c r="X822" s="3"/>
     </row>
@@ -23623,10 +23639,10 @@
       </c>
       <c r="H823" s="3"/>
       <c r="I823" s="3" t="s">
-        <v>1515</v>
+        <v>1517</v>
       </c>
       <c r="J823" s="3" t="s">
-        <v>1516</v>
+        <v>1518</v>
       </c>
       <c r="X823" s="3"/>
     </row>
@@ -23650,10 +23666,10 @@
       </c>
       <c r="H824" s="3"/>
       <c r="I824" s="3" t="s">
-        <v>1517</v>
+        <v>1519</v>
       </c>
       <c r="J824" s="3" t="s">
-        <v>1518</v>
+        <v>1520</v>
       </c>
       <c r="X824" s="3"/>
     </row>
@@ -23677,10 +23693,10 @@
       </c>
       <c r="H825" s="3"/>
       <c r="I825" s="3" t="s">
-        <v>1519</v>
+        <v>1521</v>
       </c>
       <c r="J825" s="3" t="s">
-        <v>1520</v>
+        <v>1522</v>
       </c>
       <c r="X825" s="3"/>
     </row>
@@ -23704,10 +23720,10 @@
       </c>
       <c r="H826" s="3"/>
       <c r="I826" s="3" t="s">
-        <v>1521</v>
+        <v>1523</v>
       </c>
       <c r="J826" s="3" t="s">
-        <v>1522</v>
+        <v>1524</v>
       </c>
       <c r="X826" s="3"/>
     </row>
@@ -23731,10 +23747,10 @@
       </c>
       <c r="H827" s="3"/>
       <c r="I827" s="3" t="s">
-        <v>1523</v>
+        <v>1525</v>
       </c>
       <c r="J827" s="3" t="s">
-        <v>1524</v>
+        <v>1526</v>
       </c>
       <c r="X827" s="3"/>
     </row>
@@ -23758,10 +23774,10 @@
       </c>
       <c r="H828" s="3"/>
       <c r="I828" s="3" t="s">
-        <v>1525</v>
+        <v>1527</v>
       </c>
       <c r="J828" s="3" t="s">
-        <v>1526</v>
+        <v>1528</v>
       </c>
       <c r="X828" s="3"/>
     </row>
@@ -23785,10 +23801,10 @@
       </c>
       <c r="H829" s="3"/>
       <c r="I829" s="3" t="s">
-        <v>1527</v>
+        <v>1529</v>
       </c>
       <c r="J829" s="3" t="s">
-        <v>1528</v>
+        <v>1530</v>
       </c>
       <c r="X829" s="3"/>
     </row>
@@ -23812,10 +23828,10 @@
       </c>
       <c r="H830" s="3"/>
       <c r="I830" s="3" t="s">
-        <v>1529</v>
+        <v>1531</v>
       </c>
       <c r="J830" s="3" t="s">
-        <v>1530</v>
+        <v>1532</v>
       </c>
       <c r="X830" s="3"/>
     </row>
@@ -23839,10 +23855,10 @@
       </c>
       <c r="H831" s="3"/>
       <c r="I831" s="3" t="s">
-        <v>1531</v>
+        <v>1533</v>
       </c>
       <c r="J831" s="3" t="s">
-        <v>1532</v>
+        <v>1534</v>
       </c>
       <c r="X831" s="3"/>
     </row>
@@ -23866,10 +23882,10 @@
       </c>
       <c r="H832" s="3"/>
       <c r="I832" s="3" t="s">
-        <v>1533</v>
+        <v>1535</v>
       </c>
       <c r="J832" s="3" t="s">
-        <v>1534</v>
+        <v>1536</v>
       </c>
       <c r="X832" s="3"/>
     </row>
@@ -23893,10 +23909,10 @@
       </c>
       <c r="H833" s="3"/>
       <c r="I833" s="3" t="s">
-        <v>1535</v>
+        <v>1537</v>
       </c>
       <c r="J833" s="3" t="s">
-        <v>1536</v>
+        <v>1538</v>
       </c>
       <c r="X833" s="3"/>
     </row>
@@ -23920,10 +23936,10 @@
       </c>
       <c r="H834" s="3"/>
       <c r="I834" s="3" t="s">
-        <v>1537</v>
+        <v>1539</v>
       </c>
       <c r="J834" s="3" t="s">
-        <v>1538</v>
+        <v>1540</v>
       </c>
       <c r="X834" s="3"/>
     </row>
@@ -23947,10 +23963,10 @@
       </c>
       <c r="H835" s="3"/>
       <c r="I835" s="3" t="s">
-        <v>1539</v>
+        <v>1541</v>
       </c>
       <c r="J835" s="3" t="s">
-        <v>1540</v>
+        <v>1542</v>
       </c>
       <c r="X835" s="3"/>
     </row>
@@ -23974,10 +23990,10 @@
       </c>
       <c r="H836" s="3"/>
       <c r="I836" s="3" t="s">
-        <v>1541</v>
+        <v>1543</v>
       </c>
       <c r="J836" s="3" t="s">
-        <v>1542</v>
+        <v>1544</v>
       </c>
       <c r="X836" s="3"/>
     </row>
@@ -24001,10 +24017,10 @@
       </c>
       <c r="H837" s="3"/>
       <c r="I837" s="3" t="s">
-        <v>1543</v>
+        <v>1545</v>
       </c>
       <c r="J837" s="3" t="s">
-        <v>1544</v>
+        <v>1546</v>
       </c>
       <c r="X837" s="3"/>
     </row>
@@ -24028,10 +24044,10 @@
       </c>
       <c r="H838" s="3"/>
       <c r="I838" s="3" t="s">
-        <v>1545</v>
+        <v>1547</v>
       </c>
       <c r="J838" s="3" t="s">
-        <v>1546</v>
+        <v>1548</v>
       </c>
       <c r="X838" s="3"/>
     </row>
@@ -24055,10 +24071,10 @@
       </c>
       <c r="H839" s="3"/>
       <c r="I839" s="3" t="s">
-        <v>1547</v>
+        <v>1549</v>
       </c>
       <c r="J839" s="3" t="s">
-        <v>1548</v>
+        <v>1550</v>
       </c>
       <c r="X839" s="3"/>
     </row>
@@ -24082,10 +24098,10 @@
       </c>
       <c r="H840" s="3"/>
       <c r="I840" s="3" t="s">
-        <v>1549</v>
+        <v>1551</v>
       </c>
       <c r="J840" s="3" t="s">
-        <v>1550</v>
+        <v>1552</v>
       </c>
       <c r="X840" s="3"/>
     </row>
@@ -24109,10 +24125,10 @@
       </c>
       <c r="H841" s="3"/>
       <c r="I841" s="3" t="s">
-        <v>1551</v>
+        <v>1553</v>
       </c>
       <c r="J841" s="3" t="s">
-        <v>1552</v>
+        <v>1554</v>
       </c>
       <c r="X841" s="3"/>
     </row>
@@ -24136,10 +24152,10 @@
       </c>
       <c r="H842" s="3"/>
       <c r="I842" s="3" t="s">
-        <v>1553</v>
+        <v>1555</v>
       </c>
       <c r="J842" s="3" t="s">
-        <v>1554</v>
+        <v>1556</v>
       </c>
       <c r="X842" s="3"/>
     </row>
@@ -24163,10 +24179,10 @@
       </c>
       <c r="H843" s="3"/>
       <c r="I843" s="3" t="s">
-        <v>1555</v>
+        <v>1557</v>
       </c>
       <c r="J843" s="3" t="s">
-        <v>1556</v>
+        <v>1558</v>
       </c>
       <c r="X843" s="3"/>
     </row>
@@ -24190,10 +24206,10 @@
       </c>
       <c r="H844" s="3"/>
       <c r="I844" s="3" t="s">
-        <v>1557</v>
+        <v>1559</v>
       </c>
       <c r="J844" s="3" t="s">
-        <v>1558</v>
+        <v>1560</v>
       </c>
       <c r="X844" s="3"/>
     </row>
@@ -24217,10 +24233,10 @@
       </c>
       <c r="H845" s="3"/>
       <c r="I845" s="3" t="s">
-        <v>1559</v>
+        <v>1561</v>
       </c>
       <c r="J845" s="3" t="s">
-        <v>1560</v>
+        <v>1562</v>
       </c>
       <c r="X845" s="3"/>
     </row>
@@ -24244,10 +24260,10 @@
       </c>
       <c r="H846" s="3"/>
       <c r="I846" s="3" t="s">
-        <v>1561</v>
+        <v>1563</v>
       </c>
       <c r="J846" s="3" t="s">
-        <v>1562</v>
+        <v>1564</v>
       </c>
       <c r="X846" s="3"/>
     </row>
@@ -24271,10 +24287,10 @@
       </c>
       <c r="H847" s="3"/>
       <c r="I847" s="3" t="s">
-        <v>1563</v>
+        <v>1565</v>
       </c>
       <c r="J847" s="3" t="s">
-        <v>1564</v>
+        <v>1566</v>
       </c>
       <c r="X847" s="3"/>
     </row>
@@ -24298,10 +24314,10 @@
       </c>
       <c r="H848" s="3"/>
       <c r="I848" s="3" t="s">
-        <v>1565</v>
+        <v>1567</v>
       </c>
       <c r="J848" s="3" t="s">
-        <v>1566</v>
+        <v>1568</v>
       </c>
       <c r="X848" s="3"/>
     </row>
@@ -24325,10 +24341,10 @@
       </c>
       <c r="H849" s="3"/>
       <c r="I849" s="3" t="s">
-        <v>1567</v>
+        <v>1569</v>
       </c>
       <c r="J849" s="3" t="s">
-        <v>1568</v>
+        <v>1570</v>
       </c>
       <c r="X849" s="3"/>
     </row>
@@ -24352,10 +24368,10 @@
       </c>
       <c r="H850" s="3"/>
       <c r="I850" s="3" t="s">
-        <v>1569</v>
+        <v>1571</v>
       </c>
       <c r="J850" s="3" t="s">
-        <v>1570</v>
+        <v>1572</v>
       </c>
       <c r="X850" s="3"/>
     </row>
@@ -24379,10 +24395,10 @@
       </c>
       <c r="H851" s="3"/>
       <c r="I851" s="3" t="s">
-        <v>1571</v>
+        <v>1573</v>
       </c>
       <c r="J851" s="3" t="s">
-        <v>1572</v>
+        <v>1574</v>
       </c>
       <c r="X851" s="3"/>
     </row>
@@ -24406,10 +24422,10 @@
       </c>
       <c r="H852" s="3"/>
       <c r="I852" s="3" t="s">
-        <v>1573</v>
+        <v>1575</v>
       </c>
       <c r="J852" s="3" t="s">
-        <v>1574</v>
+        <v>1576</v>
       </c>
       <c r="X852" s="3"/>
     </row>
@@ -24433,10 +24449,10 @@
       </c>
       <c r="H853" s="3"/>
       <c r="I853" s="3" t="s">
-        <v>1575</v>
+        <v>1577</v>
       </c>
       <c r="J853" s="3" t="s">
-        <v>1576</v>
+        <v>1578</v>
       </c>
       <c r="X853" s="3"/>
     </row>
@@ -24460,10 +24476,10 @@
       </c>
       <c r="H854" s="3"/>
       <c r="I854" s="3" t="s">
-        <v>1577</v>
+        <v>1579</v>
       </c>
       <c r="J854" s="3" t="s">
-        <v>1578</v>
+        <v>1580</v>
       </c>
       <c r="X854" s="3"/>
     </row>
@@ -24487,10 +24503,10 @@
       </c>
       <c r="H855" s="3"/>
       <c r="I855" s="3" t="s">
-        <v>1579</v>
+        <v>1581</v>
       </c>
       <c r="J855" s="3" t="s">
-        <v>1580</v>
+        <v>1582</v>
       </c>
       <c r="X855" s="3"/>
     </row>
@@ -24514,10 +24530,10 @@
       </c>
       <c r="H856" s="3"/>
       <c r="I856" s="3" t="s">
-        <v>1581</v>
+        <v>1583</v>
       </c>
       <c r="J856" s="3" t="s">
-        <v>1582</v>
+        <v>1584</v>
       </c>
       <c r="X856" s="3"/>
     </row>
@@ -24541,10 +24557,10 @@
       </c>
       <c r="H857" s="3"/>
       <c r="I857" s="3" t="s">
-        <v>1583</v>
+        <v>1585</v>
       </c>
       <c r="J857" s="3" t="s">
-        <v>1584</v>
+        <v>1586</v>
       </c>
       <c r="X857" s="3"/>
     </row>
@@ -24568,10 +24584,10 @@
       </c>
       <c r="H858" s="3"/>
       <c r="I858" s="3" t="s">
-        <v>1585</v>
+        <v>1587</v>
       </c>
       <c r="J858" s="3" t="s">
-        <v>1586</v>
+        <v>1588</v>
       </c>
       <c r="X858" s="3"/>
     </row>
@@ -24595,10 +24611,10 @@
       </c>
       <c r="H859" s="3"/>
       <c r="I859" s="3" t="s">
-        <v>1587</v>
+        <v>1589</v>
       </c>
       <c r="J859" s="3" t="s">
-        <v>1588</v>
+        <v>1590</v>
       </c>
       <c r="X859" s="3"/>
     </row>
@@ -24622,10 +24638,10 @@
       </c>
       <c r="H860" s="3"/>
       <c r="I860" s="3" t="s">
-        <v>1589</v>
+        <v>1591</v>
       </c>
       <c r="J860" s="3" t="s">
-        <v>1590</v>
+        <v>1592</v>
       </c>
       <c r="X860" s="3"/>
     </row>
@@ -24649,10 +24665,10 @@
       </c>
       <c r="H861" s="3"/>
       <c r="I861" s="3" t="s">
-        <v>1591</v>
+        <v>1593</v>
       </c>
       <c r="J861" s="3" t="s">
-        <v>1592</v>
+        <v>1594</v>
       </c>
       <c r="X861" s="3"/>
     </row>
@@ -24676,10 +24692,10 @@
       </c>
       <c r="H862" s="3"/>
       <c r="I862" s="3" t="s">
-        <v>1593</v>
+        <v>1595</v>
       </c>
       <c r="J862" s="3" t="s">
-        <v>1594</v>
+        <v>1596</v>
       </c>
       <c r="X862" s="3"/>
     </row>
@@ -24703,10 +24719,10 @@
       </c>
       <c r="H863" s="3"/>
       <c r="I863" s="3" t="s">
-        <v>1595</v>
+        <v>1597</v>
       </c>
       <c r="J863" s="3" t="s">
-        <v>1596</v>
+        <v>1598</v>
       </c>
       <c r="X863" s="3"/>
     </row>
@@ -24730,10 +24746,10 @@
       </c>
       <c r="H864" s="3"/>
       <c r="I864" s="3" t="s">
-        <v>1597</v>
+        <v>1599</v>
       </c>
       <c r="J864" s="3" t="s">
-        <v>1598</v>
+        <v>1600</v>
       </c>
       <c r="X864" s="3"/>
     </row>
@@ -24757,10 +24773,10 @@
       </c>
       <c r="H865" s="3"/>
       <c r="I865" s="3" t="s">
-        <v>1599</v>
+        <v>1601</v>
       </c>
       <c r="J865" s="3" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="X865" s="3"/>
     </row>
@@ -24784,10 +24800,10 @@
       </c>
       <c r="H866" s="3"/>
       <c r="I866" s="3" t="s">
-        <v>1601</v>
+        <v>1603</v>
       </c>
       <c r="J866" s="3" t="s">
-        <v>1602</v>
+        <v>1604</v>
       </c>
       <c r="X866" s="3"/>
     </row>
@@ -24811,10 +24827,10 @@
       </c>
       <c r="H867" s="3"/>
       <c r="I867" s="3" t="s">
-        <v>1603</v>
+        <v>1605</v>
       </c>
       <c r="J867" s="3" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="X867" s="3"/>
     </row>
@@ -24838,10 +24854,10 @@
       </c>
       <c r="H868" s="3"/>
       <c r="I868" s="3" t="s">
-        <v>1605</v>
+        <v>1607</v>
       </c>
       <c r="J868" s="3" t="s">
-        <v>1606</v>
+        <v>1608</v>
       </c>
       <c r="X868" s="3"/>
     </row>
@@ -24865,10 +24881,10 @@
       </c>
       <c r="H869" s="3"/>
       <c r="I869" s="3" t="s">
-        <v>1607</v>
+        <v>1609</v>
       </c>
       <c r="J869" s="3" t="s">
-        <v>1608</v>
+        <v>1610</v>
       </c>
       <c r="X869" s="3"/>
     </row>
@@ -24892,10 +24908,10 @@
       </c>
       <c r="H870" s="3"/>
       <c r="I870" s="3" t="s">
-        <v>1609</v>
+        <v>1611</v>
       </c>
       <c r="J870" s="3" t="s">
-        <v>1610</v>
+        <v>1612</v>
       </c>
       <c r="X870" s="3"/>
     </row>
@@ -24919,10 +24935,10 @@
       </c>
       <c r="H871" s="3"/>
       <c r="I871" s="3" t="s">
-        <v>1611</v>
+        <v>1613</v>
       </c>
       <c r="J871" s="3" t="s">
-        <v>1612</v>
+        <v>1614</v>
       </c>
       <c r="X871" s="3"/>
     </row>
@@ -24946,10 +24962,10 @@
       </c>
       <c r="H872" s="3"/>
       <c r="I872" s="3" t="s">
-        <v>1613</v>
+        <v>1615</v>
       </c>
       <c r="J872" s="3" t="s">
-        <v>1614</v>
+        <v>1616</v>
       </c>
       <c r="X872" s="3"/>
     </row>
@@ -24973,10 +24989,10 @@
       </c>
       <c r="H873" s="3"/>
       <c r="I873" s="3" t="s">
-        <v>1615</v>
+        <v>1617</v>
       </c>
       <c r="J873" s="3" t="s">
-        <v>1616</v>
+        <v>1618</v>
       </c>
       <c r="X873" s="3"/>
     </row>
@@ -25000,10 +25016,10 @@
       </c>
       <c r="H874" s="3"/>
       <c r="I874" s="3" t="s">
-        <v>1617</v>
+        <v>1619</v>
       </c>
       <c r="J874" s="3" t="s">
-        <v>1618</v>
+        <v>1620</v>
       </c>
       <c r="X874" s="3"/>
     </row>
@@ -25027,10 +25043,10 @@
       </c>
       <c r="H875" s="3"/>
       <c r="I875" s="3" t="s">
-        <v>1619</v>
+        <v>1621</v>
       </c>
       <c r="J875" s="3" t="s">
-        <v>1620</v>
+        <v>1622</v>
       </c>
       <c r="X875" s="3"/>
     </row>
@@ -25054,10 +25070,10 @@
       </c>
       <c r="H876" s="3"/>
       <c r="I876" s="3" t="s">
-        <v>1621</v>
+        <v>1623</v>
       </c>
       <c r="J876" s="3" t="s">
-        <v>1622</v>
+        <v>1624</v>
       </c>
       <c r="X876" s="3"/>
     </row>
@@ -25081,10 +25097,10 @@
       </c>
       <c r="H877" s="3"/>
       <c r="I877" s="3" t="s">
-        <v>1623</v>
+        <v>1625</v>
       </c>
       <c r="J877" s="3" t="s">
-        <v>1624</v>
+        <v>1626</v>
       </c>
       <c r="X877" s="3"/>
     </row>
@@ -25108,10 +25124,10 @@
       </c>
       <c r="H878" s="3"/>
       <c r="I878" s="3" t="s">
-        <v>1625</v>
+        <v>1627</v>
       </c>
       <c r="J878" s="3" t="s">
-        <v>1626</v>
+        <v>1628</v>
       </c>
       <c r="X878" s="3"/>
     </row>
@@ -25135,10 +25151,10 @@
       </c>
       <c r="H879" s="3"/>
       <c r="I879" s="3" t="s">
-        <v>1627</v>
+        <v>1629</v>
       </c>
       <c r="J879" s="3" t="s">
-        <v>1628</v>
+        <v>1630</v>
       </c>
       <c r="X879" s="3"/>
     </row>
@@ -25162,10 +25178,10 @@
       </c>
       <c r="H880" s="3"/>
       <c r="I880" s="3" t="s">
-        <v>1629</v>
+        <v>1631</v>
       </c>
       <c r="J880" s="3" t="s">
-        <v>1630</v>
+        <v>1632</v>
       </c>
       <c r="X880" s="3"/>
     </row>
@@ -25189,10 +25205,10 @@
       </c>
       <c r="H881" s="3"/>
       <c r="I881" s="3" t="s">
-        <v>1631</v>
+        <v>1633</v>
       </c>
       <c r="J881" s="3" t="s">
-        <v>1632</v>
+        <v>1634</v>
       </c>
       <c r="X881" s="3"/>
     </row>
@@ -25216,10 +25232,10 @@
       </c>
       <c r="H882" s="3"/>
       <c r="I882" s="3" t="s">
-        <v>1633</v>
+        <v>1635</v>
       </c>
       <c r="J882" s="3" t="s">
-        <v>1634</v>
+        <v>1636</v>
       </c>
       <c r="X882" s="3"/>
     </row>
@@ -25243,10 +25259,10 @@
       </c>
       <c r="H883" s="3"/>
       <c r="I883" s="3" t="s">
-        <v>1635</v>
+        <v>1637</v>
       </c>
       <c r="J883" s="3" t="s">
-        <v>1636</v>
+        <v>1638</v>
       </c>
       <c r="X883" s="3"/>
     </row>
@@ -25270,10 +25286,10 @@
       </c>
       <c r="H884" s="3"/>
       <c r="I884" s="3" t="s">
-        <v>1637</v>
+        <v>1639</v>
       </c>
       <c r="J884" s="3" t="s">
-        <v>1638</v>
+        <v>1640</v>
       </c>
       <c r="X884" s="3"/>
     </row>
@@ -25297,10 +25313,10 @@
       </c>
       <c r="H885" s="3"/>
       <c r="I885" s="3" t="s">
-        <v>1639</v>
+        <v>1641</v>
       </c>
       <c r="J885" s="3" t="s">
-        <v>1640</v>
+        <v>1642</v>
       </c>
       <c r="X885" s="3"/>
     </row>
@@ -25324,10 +25340,10 @@
       </c>
       <c r="H886" s="3"/>
       <c r="I886" s="3" t="s">
-        <v>1641</v>
+        <v>1643</v>
       </c>
       <c r="J886" s="3" t="s">
-        <v>1642</v>
+        <v>1644</v>
       </c>
       <c r="X886" s="3"/>
     </row>
@@ -25351,10 +25367,10 @@
       </c>
       <c r="H887" s="3"/>
       <c r="I887" s="3" t="s">
-        <v>1643</v>
+        <v>1645</v>
       </c>
       <c r="J887" s="3" t="s">
-        <v>1644</v>
+        <v>1646</v>
       </c>
       <c r="X887" s="3"/>
     </row>
@@ -25375,7 +25391,7 @@
       <c r="H888" s="3"/>
       <c r="I888" s="3"/>
       <c r="J888" s="3" t="s">
-        <v>1645</v>
+        <v>1647</v>
       </c>
       <c r="X888" s="3"/>
     </row>
@@ -25396,7 +25412,7 @@
       <c r="H889" s="3"/>
       <c r="I889" s="3"/>
       <c r="J889" s="3" t="s">
-        <v>1646</v>
+        <v>1648</v>
       </c>
       <c r="X889" s="3"/>
     </row>
@@ -25417,7 +25433,7 @@
       <c r="H890" s="3"/>
       <c r="I890" s="3"/>
       <c r="J890" s="3" t="s">
-        <v>1647</v>
+        <v>1649</v>
       </c>
       <c r="X890" s="3"/>
     </row>
@@ -25438,7 +25454,7 @@
       <c r="H891" s="3"/>
       <c r="I891" s="3"/>
       <c r="J891" s="3" t="s">
-        <v>1648</v>
+        <v>1650</v>
       </c>
       <c r="X891" s="3"/>
     </row>
@@ -25459,7 +25475,7 @@
       <c r="H892" s="3"/>
       <c r="I892" s="3"/>
       <c r="J892" s="3" t="s">
-        <v>1649</v>
+        <v>1651</v>
       </c>
       <c r="X892" s="3"/>
     </row>
@@ -25480,7 +25496,7 @@
       <c r="H893" s="3"/>
       <c r="I893" s="3"/>
       <c r="J893" s="3" t="s">
-        <v>1650</v>
+        <v>1652</v>
       </c>
       <c r="X893" s="3"/>
     </row>
@@ -25501,7 +25517,7 @@
       <c r="H894" s="3"/>
       <c r="I894" s="3"/>
       <c r="J894" s="3" t="s">
-        <v>1651</v>
+        <v>1653</v>
       </c>
       <c r="X894" s="3"/>
     </row>
@@ -25522,7 +25538,7 @@
       <c r="H895" s="3"/>
       <c r="I895" s="3"/>
       <c r="J895" s="3" t="s">
-        <v>1652</v>
+        <v>1654</v>
       </c>
       <c r="X895" s="3"/>
     </row>
@@ -25543,7 +25559,7 @@
       <c r="H896" s="3"/>
       <c r="I896" s="3"/>
       <c r="J896" s="3" t="s">
-        <v>1653</v>
+        <v>1655</v>
       </c>
       <c r="X896" s="3"/>
     </row>
@@ -25564,7 +25580,7 @@
       <c r="H897" s="3"/>
       <c r="I897" s="3"/>
       <c r="J897" s="3" t="s">
-        <v>1654</v>
+        <v>1656</v>
       </c>
       <c r="X897" s="3"/>
     </row>
@@ -25585,7 +25601,7 @@
       <c r="H898" s="3"/>
       <c r="I898" s="3"/>
       <c r="J898" s="3" t="s">
-        <v>1655</v>
+        <v>1657</v>
       </c>
       <c r="X898" s="3"/>
     </row>
@@ -25606,7 +25622,7 @@
       <c r="H899" s="3"/>
       <c r="I899" s="3"/>
       <c r="J899" s="3" t="s">
-        <v>1656</v>
+        <v>1658</v>
       </c>
       <c r="X899" s="3"/>
     </row>
@@ -25627,7 +25643,7 @@
       <c r="H900" s="3"/>
       <c r="I900" s="3"/>
       <c r="J900" s="3" t="s">
-        <v>1657</v>
+        <v>1659</v>
       </c>
       <c r="X900" s="3"/>
     </row>
@@ -25648,7 +25664,7 @@
       <c r="H901" s="3"/>
       <c r="I901" s="3"/>
       <c r="J901" s="3" t="s">
-        <v>1658</v>
+        <v>1660</v>
       </c>
       <c r="X901" s="3"/>
     </row>
@@ -25669,7 +25685,7 @@
       <c r="H902" s="3"/>
       <c r="I902" s="3"/>
       <c r="J902" s="3" t="s">
-        <v>1659</v>
+        <v>1661</v>
       </c>
       <c r="X902" s="3"/>
     </row>
@@ -25690,7 +25706,7 @@
       <c r="H903" s="3"/>
       <c r="I903" s="3"/>
       <c r="J903" s="3" t="s">
-        <v>1660</v>
+        <v>1662</v>
       </c>
       <c r="X903" s="3"/>
     </row>
@@ -25711,7 +25727,7 @@
       <c r="H904" s="3"/>
       <c r="I904" s="3"/>
       <c r="J904" s="3" t="s">
-        <v>1661</v>
+        <v>1663</v>
       </c>
       <c r="X904" s="3"/>
     </row>
@@ -25732,7 +25748,7 @@
       <c r="H905" s="3"/>
       <c r="I905" s="3"/>
       <c r="J905" s="3" t="s">
-        <v>1662</v>
+        <v>1664</v>
       </c>
       <c r="X905" s="3"/>
     </row>
@@ -25753,7 +25769,7 @@
       <c r="H906" s="3"/>
       <c r="I906" s="3"/>
       <c r="J906" s="3" t="s">
-        <v>1663</v>
+        <v>1665</v>
       </c>
       <c r="X906" s="3"/>
     </row>
@@ -25774,7 +25790,7 @@
       <c r="H907" s="3"/>
       <c r="I907" s="3"/>
       <c r="J907" s="3" t="s">
-        <v>1664</v>
+        <v>1666</v>
       </c>
       <c r="X907" s="3"/>
     </row>
@@ -25795,7 +25811,7 @@
       <c r="H908" s="3"/>
       <c r="I908" s="3"/>
       <c r="J908" s="3" t="s">
-        <v>1665</v>
+        <v>1667</v>
       </c>
       <c r="X908" s="3"/>
     </row>
@@ -25816,7 +25832,7 @@
       <c r="H909" s="3"/>
       <c r="I909" s="3"/>
       <c r="J909" s="3" t="s">
-        <v>1666</v>
+        <v>1668</v>
       </c>
       <c r="X909" s="3"/>
     </row>
@@ -25837,7 +25853,7 @@
       <c r="H910" s="3"/>
       <c r="I910" s="3"/>
       <c r="J910" s="3" t="s">
-        <v>1667</v>
+        <v>1669</v>
       </c>
       <c r="X910" s="3"/>
     </row>
@@ -25858,7 +25874,7 @@
       <c r="H911" s="3"/>
       <c r="I911" s="3"/>
       <c r="J911" s="3" t="s">
-        <v>1668</v>
+        <v>1670</v>
       </c>
       <c r="X911" s="3"/>
     </row>
@@ -25875,17 +25891,17 @@
       <c r="D912" s="3"/>
       <c r="E912" s="3"/>
       <c r="F912" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G912" s="3">
         <v>5000</v>
       </c>
       <c r="H912" s="3"/>
       <c r="I912" s="3" t="s">
-        <v>1670</v>
+        <v>1672</v>
       </c>
       <c r="J912" s="3" t="s">
-        <v>1671</v>
+        <v>1673</v>
       </c>
       <c r="X912" s="3"/>
     </row>
@@ -25902,17 +25918,17 @@
       <c r="D913" s="3"/>
       <c r="E913" s="3"/>
       <c r="F913" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G913" s="3">
         <v>5000</v>
       </c>
       <c r="H913" s="3"/>
       <c r="I913" s="3" t="s">
-        <v>1672</v>
+        <v>1674</v>
       </c>
       <c r="J913" s="3" t="s">
-        <v>1673</v>
+        <v>1675</v>
       </c>
       <c r="X913" s="3"/>
     </row>
@@ -25929,17 +25945,17 @@
       <c r="D914" s="3"/>
       <c r="E914" s="3"/>
       <c r="F914" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G914" s="3">
         <v>5000</v>
       </c>
       <c r="H914" s="3"/>
       <c r="I914" s="3" t="s">
-        <v>1674</v>
+        <v>1676</v>
       </c>
       <c r="J914" s="3" t="s">
-        <v>1675</v>
+        <v>1677</v>
       </c>
       <c r="X914" s="3"/>
     </row>
@@ -25956,17 +25972,17 @@
       <c r="D915" s="3"/>
       <c r="E915" s="3"/>
       <c r="F915" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G915" s="3">
         <v>5000</v>
       </c>
       <c r="H915" s="3"/>
       <c r="I915" s="3" t="s">
-        <v>1676</v>
+        <v>1678</v>
       </c>
       <c r="J915" s="3" t="s">
-        <v>1677</v>
+        <v>1679</v>
       </c>
       <c r="X915" s="3"/>
     </row>
@@ -25983,17 +25999,17 @@
       <c r="D916" s="3"/>
       <c r="E916" s="3"/>
       <c r="F916" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G916" s="3">
         <v>5000</v>
       </c>
       <c r="H916" s="3"/>
       <c r="I916" s="3" t="s">
-        <v>1678</v>
+        <v>1680</v>
       </c>
       <c r="J916" s="3" t="s">
-        <v>1679</v>
+        <v>1681</v>
       </c>
       <c r="X916" s="3"/>
     </row>
@@ -26010,17 +26026,17 @@
       <c r="D917" s="3"/>
       <c r="E917" s="3"/>
       <c r="F917" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G917" s="3">
         <v>5000</v>
       </c>
       <c r="H917" s="3"/>
       <c r="I917" s="3" t="s">
-        <v>1680</v>
+        <v>1682</v>
       </c>
       <c r="J917" s="3" t="s">
-        <v>1681</v>
+        <v>1683</v>
       </c>
       <c r="X917" s="3"/>
     </row>
@@ -26037,17 +26053,17 @@
       <c r="D918" s="3"/>
       <c r="E918" s="3"/>
       <c r="F918" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G918" s="3">
         <v>5000</v>
       </c>
       <c r="H918" s="3"/>
       <c r="I918" s="3" t="s">
-        <v>1682</v>
+        <v>1684</v>
       </c>
       <c r="J918" s="3" t="s">
-        <v>1683</v>
+        <v>1685</v>
       </c>
       <c r="X918" s="3"/>
     </row>
@@ -26068,7 +26084,7 @@
       <c r="H919" s="3"/>
       <c r="I919" s="3"/>
       <c r="J919" s="3" t="s">
-        <v>1684</v>
+        <v>1686</v>
       </c>
       <c r="X919" s="3"/>
     </row>
@@ -26085,17 +26101,17 @@
       <c r="D920" s="3"/>
       <c r="E920" s="3"/>
       <c r="F920" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G920" s="3">
         <v>5000</v>
       </c>
       <c r="H920" s="3"/>
       <c r="I920" s="3" t="s">
-        <v>1685</v>
+        <v>1687</v>
       </c>
       <c r="J920" s="3" t="s">
-        <v>1686</v>
+        <v>1688</v>
       </c>
       <c r="X920" s="3"/>
     </row>
@@ -26112,17 +26128,17 @@
       <c r="D921" s="3"/>
       <c r="E921" s="3"/>
       <c r="F921" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G921" s="3">
         <v>5000</v>
       </c>
       <c r="H921" s="3"/>
       <c r="I921" s="3" t="s">
-        <v>1687</v>
+        <v>1689</v>
       </c>
       <c r="J921" s="3" t="s">
-        <v>1688</v>
+        <v>1690</v>
       </c>
       <c r="X921" s="3"/>
     </row>
@@ -26139,17 +26155,17 @@
       <c r="D922" s="3"/>
       <c r="E922" s="3"/>
       <c r="F922" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G922" s="3">
         <v>5000</v>
       </c>
       <c r="H922" s="3"/>
       <c r="I922" s="3" t="s">
-        <v>1689</v>
+        <v>1691</v>
       </c>
       <c r="J922" s="3" t="s">
-        <v>1690</v>
+        <v>1692</v>
       </c>
       <c r="X922" s="3"/>
     </row>
@@ -26166,17 +26182,17 @@
       <c r="D923" s="3"/>
       <c r="E923" s="3"/>
       <c r="F923" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G923" s="3">
         <v>5000</v>
       </c>
       <c r="H923" s="3"/>
       <c r="I923" s="3" t="s">
-        <v>1691</v>
+        <v>1693</v>
       </c>
       <c r="J923" s="3" t="s">
-        <v>1692</v>
+        <v>1694</v>
       </c>
       <c r="X923" s="3"/>
     </row>
@@ -26193,17 +26209,17 @@
       <c r="D924" s="3"/>
       <c r="E924" s="3"/>
       <c r="F924" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G924" s="3">
         <v>5000</v>
       </c>
       <c r="H924" s="3"/>
       <c r="I924" s="3" t="s">
-        <v>1693</v>
+        <v>1695</v>
       </c>
       <c r="J924" s="3" t="s">
-        <v>1694</v>
+        <v>1696</v>
       </c>
       <c r="X924" s="3"/>
     </row>
@@ -26220,17 +26236,17 @@
       <c r="D925" s="3"/>
       <c r="E925" s="3"/>
       <c r="F925" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G925" s="3">
         <v>5000</v>
       </c>
       <c r="H925" s="3"/>
       <c r="I925" s="3" t="s">
-        <v>1695</v>
+        <v>1697</v>
       </c>
       <c r="J925" s="3" t="s">
-        <v>1696</v>
+        <v>1698</v>
       </c>
       <c r="X925" s="3"/>
     </row>
@@ -26247,17 +26263,17 @@
       <c r="D926" s="3"/>
       <c r="E926" s="3"/>
       <c r="F926" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G926" s="3">
         <v>5000</v>
       </c>
       <c r="H926" s="3"/>
       <c r="I926" s="3" t="s">
-        <v>1697</v>
+        <v>1699</v>
       </c>
       <c r="J926" s="3" t="s">
-        <v>1698</v>
+        <v>1700</v>
       </c>
       <c r="X926" s="3"/>
     </row>
@@ -26274,17 +26290,17 @@
       <c r="D927" s="3"/>
       <c r="E927" s="3"/>
       <c r="F927" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G927" s="3">
         <v>5000</v>
       </c>
       <c r="H927" s="3"/>
       <c r="I927" s="3" t="s">
-        <v>1699</v>
+        <v>1701</v>
       </c>
       <c r="J927" s="3" t="s">
-        <v>1700</v>
+        <v>1702</v>
       </c>
       <c r="X927" s="3"/>
     </row>
@@ -26301,17 +26317,17 @@
       <c r="D928" s="3"/>
       <c r="E928" s="3"/>
       <c r="F928" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G928" s="3">
         <v>5000</v>
       </c>
       <c r="H928" s="3"/>
       <c r="I928" s="3" t="s">
-        <v>1701</v>
+        <v>1703</v>
       </c>
       <c r="J928" s="3" t="s">
-        <v>1702</v>
+        <v>1704</v>
       </c>
       <c r="X928" s="3"/>
     </row>
@@ -26328,17 +26344,17 @@
       <c r="D929" s="3"/>
       <c r="E929" s="3"/>
       <c r="F929" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G929" s="3">
         <v>5000</v>
       </c>
       <c r="H929" s="3"/>
       <c r="I929" s="3" t="s">
-        <v>1703</v>
+        <v>1705</v>
       </c>
       <c r="J929" s="3" t="s">
-        <v>1704</v>
+        <v>1706</v>
       </c>
       <c r="X929" s="3"/>
     </row>
@@ -26355,17 +26371,17 @@
       <c r="D930" s="3"/>
       <c r="E930" s="3"/>
       <c r="F930" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G930" s="3">
         <v>5000</v>
       </c>
       <c r="H930" s="3"/>
       <c r="I930" s="3" t="s">
-        <v>1705</v>
+        <v>1707</v>
       </c>
       <c r="J930" s="3" t="s">
-        <v>1706</v>
+        <v>1708</v>
       </c>
       <c r="X930" s="3"/>
     </row>
@@ -26382,17 +26398,17 @@
       <c r="D931" s="3"/>
       <c r="E931" s="3"/>
       <c r="F931" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G931" s="3">
         <v>2700</v>
       </c>
       <c r="H931" s="3"/>
       <c r="I931" s="3" t="s">
-        <v>1707</v>
+        <v>1709</v>
       </c>
       <c r="J931" s="3" t="s">
-        <v>1708</v>
+        <v>1710</v>
       </c>
       <c r="X931" s="3"/>
     </row>
@@ -26409,17 +26425,17 @@
       <c r="D932" s="3"/>
       <c r="E932" s="3"/>
       <c r="F932" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G932" s="3">
         <v>5000</v>
       </c>
       <c r="H932" s="3"/>
       <c r="I932" s="3" t="s">
-        <v>1709</v>
+        <v>1711</v>
       </c>
       <c r="J932" s="3" t="s">
-        <v>1710</v>
+        <v>1712</v>
       </c>
       <c r="X932" s="3"/>
     </row>
@@ -26436,17 +26452,17 @@
       <c r="D933" s="3"/>
       <c r="E933" s="3"/>
       <c r="F933" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G933" s="3">
         <v>5000</v>
       </c>
       <c r="H933" s="3"/>
       <c r="I933" s="3" t="s">
-        <v>1711</v>
+        <v>1713</v>
       </c>
       <c r="J933" s="3" t="s">
-        <v>1712</v>
+        <v>1714</v>
       </c>
       <c r="X933" s="3"/>
     </row>
@@ -26463,17 +26479,17 @@
       <c r="D934" s="3"/>
       <c r="E934" s="3"/>
       <c r="F934" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G934" s="3">
         <v>5000</v>
       </c>
       <c r="H934" s="3"/>
       <c r="I934" s="3" t="s">
-        <v>1713</v>
+        <v>1715</v>
       </c>
       <c r="J934" s="3" t="s">
-        <v>1714</v>
+        <v>1716</v>
       </c>
       <c r="X934" s="3"/>
     </row>
@@ -26490,17 +26506,17 @@
       <c r="D935" s="3"/>
       <c r="E935" s="3"/>
       <c r="F935" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G935" s="3">
         <v>5000</v>
       </c>
       <c r="H935" s="3"/>
       <c r="I935" s="3" t="s">
-        <v>1715</v>
+        <v>1717</v>
       </c>
       <c r="J935" s="3" t="s">
-        <v>1716</v>
+        <v>1718</v>
       </c>
       <c r="X935" s="3"/>
     </row>
@@ -26517,17 +26533,17 @@
       <c r="D936" s="3"/>
       <c r="E936" s="3"/>
       <c r="F936" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G936" s="3">
         <v>5000</v>
       </c>
       <c r="H936" s="3"/>
       <c r="I936" s="3" t="s">
-        <v>1717</v>
+        <v>1719</v>
       </c>
       <c r="J936" s="3" t="s">
-        <v>1718</v>
+        <v>1720</v>
       </c>
       <c r="X936" s="3"/>
     </row>
@@ -26544,17 +26560,17 @@
       <c r="D937" s="3"/>
       <c r="E937" s="3"/>
       <c r="F937" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G937" s="3">
         <v>5000</v>
       </c>
       <c r="H937" s="3"/>
       <c r="I937" s="3" t="s">
-        <v>1719</v>
+        <v>1721</v>
       </c>
       <c r="J937" s="3" t="s">
-        <v>1720</v>
+        <v>1722</v>
       </c>
       <c r="X937" s="3"/>
     </row>
@@ -26571,17 +26587,17 @@
       <c r="D938" s="3"/>
       <c r="E938" s="3"/>
       <c r="F938" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G938" s="3">
         <v>5000</v>
       </c>
       <c r="H938" s="3"/>
       <c r="I938" s="3" t="s">
-        <v>1721</v>
+        <v>1723</v>
       </c>
       <c r="J938" s="3" t="s">
-        <v>1722</v>
+        <v>1724</v>
       </c>
       <c r="X938" s="3"/>
     </row>
@@ -26598,17 +26614,17 @@
       <c r="D939" s="3"/>
       <c r="E939" s="3"/>
       <c r="F939" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G939" s="3">
         <v>5000</v>
       </c>
       <c r="H939" s="3"/>
       <c r="I939" s="3" t="s">
-        <v>1723</v>
+        <v>1725</v>
       </c>
       <c r="J939" s="3" t="s">
-        <v>1724</v>
+        <v>1726</v>
       </c>
       <c r="X939" s="3"/>
     </row>
@@ -26625,17 +26641,17 @@
       <c r="D940" s="3"/>
       <c r="E940" s="3"/>
       <c r="F940" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G940" s="3">
         <v>5000</v>
       </c>
       <c r="H940" s="3"/>
       <c r="I940" s="3" t="s">
-        <v>1725</v>
+        <v>1727</v>
       </c>
       <c r="J940" s="3" t="s">
-        <v>1726</v>
+        <v>1728</v>
       </c>
       <c r="X940" s="3"/>
     </row>
@@ -26652,17 +26668,17 @@
       <c r="D941" s="3"/>
       <c r="E941" s="3"/>
       <c r="F941" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G941" s="3">
         <v>5000</v>
       </c>
       <c r="H941" s="3"/>
       <c r="I941" s="3" t="s">
-        <v>1727</v>
+        <v>1729</v>
       </c>
       <c r="J941" s="3" t="s">
-        <v>1728</v>
+        <v>1730</v>
       </c>
       <c r="X941" s="3"/>
     </row>
@@ -26679,17 +26695,17 @@
       <c r="D942" s="3"/>
       <c r="E942" s="3"/>
       <c r="F942" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G942" s="3">
         <v>5000</v>
       </c>
       <c r="H942" s="3"/>
       <c r="I942" s="3" t="s">
-        <v>1729</v>
+        <v>1731</v>
       </c>
       <c r="J942" s="3" t="s">
-        <v>1730</v>
+        <v>1732</v>
       </c>
       <c r="X942" s="3"/>
     </row>
@@ -26706,17 +26722,17 @@
       <c r="D943" s="3"/>
       <c r="E943" s="3"/>
       <c r="F943" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G943" s="3">
         <v>5000</v>
       </c>
       <c r="H943" s="3"/>
       <c r="I943" s="3" t="s">
-        <v>1731</v>
+        <v>1733</v>
       </c>
       <c r="J943" s="3" t="s">
-        <v>1732</v>
+        <v>1734</v>
       </c>
       <c r="X943" s="3"/>
     </row>
@@ -26733,17 +26749,17 @@
       <c r="D944" s="3"/>
       <c r="E944" s="3"/>
       <c r="F944" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G944" s="3">
         <v>5000</v>
       </c>
       <c r="H944" s="3"/>
       <c r="I944" s="3" t="s">
-        <v>1733</v>
+        <v>1735</v>
       </c>
       <c r="J944" s="3" t="s">
-        <v>1734</v>
+        <v>1736</v>
       </c>
       <c r="X944" s="3"/>
     </row>
@@ -26760,17 +26776,17 @@
       <c r="D945" s="3"/>
       <c r="E945" s="3"/>
       <c r="F945" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G945" s="3">
         <v>5000</v>
       </c>
       <c r="H945" s="3"/>
       <c r="I945" s="3" t="s">
-        <v>1735</v>
+        <v>1737</v>
       </c>
       <c r="J945" s="3" t="s">
-        <v>1736</v>
+        <v>1738</v>
       </c>
       <c r="X945" s="3"/>
     </row>
@@ -26787,17 +26803,17 @@
       <c r="D946" s="3"/>
       <c r="E946" s="3"/>
       <c r="F946" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G946" s="3">
         <v>5000</v>
       </c>
       <c r="H946" s="3"/>
       <c r="I946" s="3" t="s">
-        <v>1737</v>
+        <v>1739</v>
       </c>
       <c r="J946" s="3" t="s">
-        <v>1738</v>
+        <v>1740</v>
       </c>
       <c r="X946" s="3"/>
     </row>
@@ -26814,17 +26830,17 @@
       <c r="D947" s="3"/>
       <c r="E947" s="3"/>
       <c r="F947" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G947" s="3">
         <v>5000</v>
       </c>
       <c r="H947" s="3"/>
       <c r="I947" s="3" t="s">
-        <v>1739</v>
+        <v>1741</v>
       </c>
       <c r="J947" s="3" t="s">
-        <v>1740</v>
+        <v>1742</v>
       </c>
       <c r="X947" s="3"/>
     </row>
@@ -26841,17 +26857,17 @@
       <c r="D948" s="3"/>
       <c r="E948" s="3"/>
       <c r="F948" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G948" s="3">
         <v>5000</v>
       </c>
       <c r="H948" s="3"/>
       <c r="I948" s="3" t="s">
-        <v>1741</v>
+        <v>1743</v>
       </c>
       <c r="J948" s="3" t="s">
-        <v>1742</v>
+        <v>1744</v>
       </c>
       <c r="X948" s="3"/>
     </row>
@@ -26868,17 +26884,17 @@
       <c r="D949" s="3"/>
       <c r="E949" s="3"/>
       <c r="F949" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G949" s="3">
         <v>5000</v>
       </c>
       <c r="H949" s="3"/>
       <c r="I949" s="3" t="s">
-        <v>1743</v>
+        <v>1745</v>
       </c>
       <c r="J949" s="3" t="s">
-        <v>1744</v>
+        <v>1746</v>
       </c>
       <c r="X949" s="3"/>
     </row>
@@ -26895,17 +26911,17 @@
       <c r="D950" s="3"/>
       <c r="E950" s="3"/>
       <c r="F950" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G950" s="3">
         <v>5000</v>
       </c>
       <c r="H950" s="3"/>
       <c r="I950" s="3" t="s">
-        <v>1745</v>
+        <v>1747</v>
       </c>
       <c r="J950" s="3" t="s">
-        <v>1746</v>
+        <v>1748</v>
       </c>
       <c r="X950" s="3"/>
     </row>
@@ -26922,17 +26938,17 @@
       <c r="D951" s="3"/>
       <c r="E951" s="3"/>
       <c r="F951" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G951" s="3">
         <v>5000</v>
       </c>
       <c r="H951" s="3"/>
       <c r="I951" s="3" t="s">
-        <v>1747</v>
+        <v>1749</v>
       </c>
       <c r="J951" s="3" t="s">
-        <v>1748</v>
+        <v>1750</v>
       </c>
       <c r="X951" s="3"/>
     </row>
@@ -26949,17 +26965,17 @@
       <c r="D952" s="3"/>
       <c r="E952" s="3"/>
       <c r="F952" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G952" s="3">
         <v>5000</v>
       </c>
       <c r="H952" s="3"/>
       <c r="I952" s="3" t="s">
-        <v>1749</v>
+        <v>1751</v>
       </c>
       <c r="J952" s="3" t="s">
-        <v>1750</v>
+        <v>1752</v>
       </c>
       <c r="X952" s="3"/>
     </row>
@@ -26976,17 +26992,17 @@
       <c r="D953" s="3"/>
       <c r="E953" s="3"/>
       <c r="F953" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G953" s="3">
         <v>5000</v>
       </c>
       <c r="H953" s="3"/>
       <c r="I953" s="3" t="s">
-        <v>1751</v>
+        <v>1753</v>
       </c>
       <c r="J953" s="3" t="s">
-        <v>1752</v>
+        <v>1754</v>
       </c>
       <c r="X953" s="3"/>
     </row>
@@ -27003,17 +27019,17 @@
       <c r="D954" s="3"/>
       <c r="E954" s="3"/>
       <c r="F954" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G954" s="3">
         <v>5000</v>
       </c>
       <c r="H954" s="3"/>
       <c r="I954" s="3" t="s">
-        <v>1753</v>
+        <v>1755</v>
       </c>
       <c r="J954" s="3" t="s">
-        <v>1754</v>
+        <v>1756</v>
       </c>
       <c r="X954" s="3"/>
     </row>
@@ -27030,17 +27046,17 @@
       <c r="D955" s="3"/>
       <c r="E955" s="3"/>
       <c r="F955" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G955" s="3">
         <v>5000</v>
       </c>
       <c r="H955" s="3"/>
       <c r="I955" s="3" t="s">
-        <v>1755</v>
+        <v>1757</v>
       </c>
       <c r="J955" s="3" t="s">
-        <v>1756</v>
+        <v>1758</v>
       </c>
       <c r="X955" s="3"/>
     </row>
@@ -27057,17 +27073,17 @@
       <c r="D956" s="3"/>
       <c r="E956" s="3"/>
       <c r="F956" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G956" s="3">
         <v>5000</v>
       </c>
       <c r="H956" s="3"/>
       <c r="I956" s="3" t="s">
-        <v>1757</v>
+        <v>1759</v>
       </c>
       <c r="J956" s="3" t="s">
-        <v>1758</v>
+        <v>1760</v>
       </c>
       <c r="X956" s="3"/>
     </row>
@@ -27084,17 +27100,17 @@
       <c r="D957" s="3"/>
       <c r="E957" s="3"/>
       <c r="F957" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G957" s="3">
         <v>5000</v>
       </c>
       <c r="H957" s="3"/>
       <c r="I957" s="3" t="s">
-        <v>1759</v>
+        <v>1761</v>
       </c>
       <c r="J957" s="3" t="s">
-        <v>1760</v>
+        <v>1762</v>
       </c>
       <c r="X957" s="3"/>
     </row>
@@ -27111,17 +27127,17 @@
       <c r="D958" s="3"/>
       <c r="E958" s="3"/>
       <c r="F958" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G958" s="3">
         <v>5000</v>
       </c>
       <c r="H958" s="3"/>
       <c r="I958" s="3" t="s">
-        <v>1761</v>
+        <v>1763</v>
       </c>
       <c r="J958" s="3" t="s">
-        <v>1762</v>
+        <v>1764</v>
       </c>
       <c r="X958" s="3"/>
     </row>
@@ -27138,17 +27154,17 @@
       <c r="D959" s="3"/>
       <c r="E959" s="3"/>
       <c r="F959" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G959" s="3">
         <v>5000</v>
       </c>
       <c r="H959" s="3"/>
       <c r="I959" s="3" t="s">
-        <v>1763</v>
+        <v>1765</v>
       </c>
       <c r="J959" s="3" t="s">
-        <v>1764</v>
+        <v>1766</v>
       </c>
       <c r="X959" s="3"/>
     </row>
@@ -27165,17 +27181,17 @@
       <c r="D960" s="3"/>
       <c r="E960" s="3"/>
       <c r="F960" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G960" s="3">
         <v>5000</v>
       </c>
       <c r="H960" s="3"/>
       <c r="I960" s="3" t="s">
-        <v>1765</v>
+        <v>1767</v>
       </c>
       <c r="J960" s="3" t="s">
-        <v>1766</v>
+        <v>1768</v>
       </c>
       <c r="X960" s="3"/>
     </row>
@@ -27192,17 +27208,17 @@
       <c r="D961" s="3"/>
       <c r="E961" s="3"/>
       <c r="F961" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G961" s="3">
         <v>5000</v>
       </c>
       <c r="H961" s="3"/>
       <c r="I961" s="3" t="s">
-        <v>1767</v>
+        <v>1769</v>
       </c>
       <c r="J961" s="3" t="s">
-        <v>1768</v>
+        <v>1770</v>
       </c>
       <c r="X961" s="3"/>
     </row>
@@ -27219,17 +27235,17 @@
       <c r="D962" s="3"/>
       <c r="E962" s="3"/>
       <c r="F962" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G962" s="3">
         <v>5000</v>
       </c>
       <c r="H962" s="3"/>
       <c r="I962" s="3" t="s">
-        <v>1769</v>
+        <v>1771</v>
       </c>
       <c r="J962" s="3" t="s">
-        <v>1770</v>
+        <v>1772</v>
       </c>
       <c r="X962" s="3"/>
     </row>
@@ -27246,17 +27262,17 @@
       <c r="D963" s="3"/>
       <c r="E963" s="3"/>
       <c r="F963" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G963" s="3">
         <v>5000</v>
       </c>
       <c r="H963" s="3"/>
       <c r="I963" s="3" t="s">
-        <v>1771</v>
+        <v>1773</v>
       </c>
       <c r="J963" s="3" t="s">
-        <v>1772</v>
+        <v>1774</v>
       </c>
       <c r="X963" s="3"/>
     </row>
@@ -27273,17 +27289,17 @@
       <c r="D964" s="3"/>
       <c r="E964" s="3"/>
       <c r="F964" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G964" s="3">
         <v>5000</v>
       </c>
       <c r="H964" s="3"/>
       <c r="I964" s="3" t="s">
-        <v>1773</v>
+        <v>1775</v>
       </c>
       <c r="J964" s="3" t="s">
-        <v>1774</v>
+        <v>1776</v>
       </c>
       <c r="X964" s="3"/>
     </row>
@@ -27300,17 +27316,17 @@
       <c r="D965" s="3"/>
       <c r="E965" s="3"/>
       <c r="F965" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G965" s="3">
         <v>5000</v>
       </c>
       <c r="H965" s="3"/>
       <c r="I965" s="3" t="s">
-        <v>1775</v>
+        <v>1777</v>
       </c>
       <c r="J965" s="3" t="s">
-        <v>1776</v>
+        <v>1778</v>
       </c>
       <c r="X965" s="3"/>
     </row>
@@ -27327,17 +27343,17 @@
       <c r="D966" s="3"/>
       <c r="E966" s="3"/>
       <c r="F966" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G966" s="3">
         <v>5000</v>
       </c>
       <c r="H966" s="3"/>
       <c r="I966" s="3" t="s">
-        <v>1777</v>
+        <v>1779</v>
       </c>
       <c r="J966" s="3" t="s">
-        <v>1778</v>
+        <v>1780</v>
       </c>
       <c r="X966" s="3"/>
     </row>
@@ -27354,17 +27370,17 @@
       <c r="D967" s="3"/>
       <c r="E967" s="3"/>
       <c r="F967" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G967" s="3">
         <v>5000</v>
       </c>
       <c r="H967" s="3"/>
       <c r="I967" s="3" t="s">
-        <v>1779</v>
+        <v>1781</v>
       </c>
       <c r="J967" s="3" t="s">
-        <v>1780</v>
+        <v>1782</v>
       </c>
       <c r="X967" s="3"/>
     </row>
@@ -27381,17 +27397,17 @@
       <c r="D968" s="3"/>
       <c r="E968" s="3"/>
       <c r="F968" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G968" s="3">
         <v>5000</v>
       </c>
       <c r="H968" s="3"/>
       <c r="I968" s="3" t="s">
-        <v>1781</v>
+        <v>1783</v>
       </c>
       <c r="J968" s="3" t="s">
-        <v>1782</v>
+        <v>1784</v>
       </c>
       <c r="X968" s="3"/>
     </row>
@@ -27408,17 +27424,17 @@
       <c r="D969" s="3"/>
       <c r="E969" s="3"/>
       <c r="F969" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G969" s="3">
         <v>5000</v>
       </c>
       <c r="H969" s="3"/>
       <c r="I969" s="3" t="s">
-        <v>1783</v>
+        <v>1785</v>
       </c>
       <c r="J969" s="3" t="s">
-        <v>1784</v>
+        <v>1786</v>
       </c>
       <c r="X969" s="3"/>
     </row>
@@ -27435,17 +27451,17 @@
       <c r="D970" s="3"/>
       <c r="E970" s="3"/>
       <c r="F970" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G970" s="3">
         <v>5000</v>
       </c>
       <c r="H970" s="3"/>
       <c r="I970" s="3" t="s">
-        <v>1785</v>
+        <v>1787</v>
       </c>
       <c r="J970" s="3" t="s">
-        <v>1786</v>
+        <v>1788</v>
       </c>
       <c r="X970" s="3"/>
     </row>
@@ -27462,17 +27478,17 @@
       <c r="D971" s="3"/>
       <c r="E971" s="3"/>
       <c r="F971" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G971" s="3">
         <v>5000</v>
       </c>
       <c r="H971" s="3"/>
       <c r="I971" s="3" t="s">
-        <v>1787</v>
+        <v>1789</v>
       </c>
       <c r="J971" s="3" t="s">
-        <v>1788</v>
+        <v>1790</v>
       </c>
       <c r="X971" s="3"/>
     </row>
@@ -27489,17 +27505,17 @@
       <c r="D972" s="3"/>
       <c r="E972" s="3"/>
       <c r="F972" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G972" s="3">
         <v>5000</v>
       </c>
       <c r="H972" s="3"/>
       <c r="I972" s="3" t="s">
-        <v>1789</v>
+        <v>1791</v>
       </c>
       <c r="J972" s="3" t="s">
-        <v>1790</v>
+        <v>1792</v>
       </c>
       <c r="X972" s="3"/>
     </row>
@@ -27516,17 +27532,17 @@
       <c r="D973" s="3"/>
       <c r="E973" s="3"/>
       <c r="F973" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G973" s="3">
         <v>5000</v>
       </c>
       <c r="H973" s="3"/>
       <c r="I973" s="3" t="s">
-        <v>1791</v>
+        <v>1793</v>
       </c>
       <c r="J973" s="3" t="s">
-        <v>1792</v>
+        <v>1794</v>
       </c>
       <c r="X973" s="3"/>
     </row>
@@ -27543,17 +27559,17 @@
       <c r="D974" s="3"/>
       <c r="E974" s="3"/>
       <c r="F974" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G974" s="3">
         <v>5000</v>
       </c>
       <c r="H974" s="3"/>
       <c r="I974" s="3" t="s">
-        <v>1793</v>
+        <v>1795</v>
       </c>
       <c r="J974" s="3" t="s">
-        <v>1794</v>
+        <v>1796</v>
       </c>
       <c r="X974" s="3"/>
     </row>
@@ -27570,17 +27586,17 @@
       <c r="D975" s="3"/>
       <c r="E975" s="3"/>
       <c r="F975" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G975" s="3">
         <v>5000</v>
       </c>
       <c r="H975" s="3"/>
       <c r="I975" s="3" t="s">
-        <v>1795</v>
+        <v>1797</v>
       </c>
       <c r="J975" s="3" t="s">
-        <v>1796</v>
+        <v>1798</v>
       </c>
       <c r="X975" s="3"/>
     </row>
@@ -27597,17 +27613,17 @@
       <c r="D976" s="3"/>
       <c r="E976" s="3"/>
       <c r="F976" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G976" s="3">
         <v>5000</v>
       </c>
       <c r="H976" s="3"/>
       <c r="I976" s="3" t="s">
-        <v>1797</v>
+        <v>1799</v>
       </c>
       <c r="J976" s="3" t="s">
-        <v>1798</v>
+        <v>1800</v>
       </c>
       <c r="X976" s="3"/>
     </row>
@@ -27624,17 +27640,17 @@
       <c r="D977" s="3"/>
       <c r="E977" s="3"/>
       <c r="F977" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G977" s="3">
         <v>5000</v>
       </c>
       <c r="H977" s="3"/>
       <c r="I977" s="3" t="s">
-        <v>1799</v>
+        <v>1801</v>
       </c>
       <c r="J977" s="3" t="s">
-        <v>1800</v>
+        <v>1802</v>
       </c>
       <c r="X977" s="3"/>
     </row>
@@ -27651,17 +27667,17 @@
       <c r="D978" s="3"/>
       <c r="E978" s="3"/>
       <c r="F978" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G978" s="3">
         <v>5000</v>
       </c>
       <c r="H978" s="3"/>
       <c r="I978" s="3" t="s">
-        <v>1801</v>
+        <v>1803</v>
       </c>
       <c r="J978" s="3" t="s">
-        <v>1802</v>
+        <v>1804</v>
       </c>
       <c r="X978" s="3"/>
     </row>
@@ -27678,17 +27694,17 @@
       <c r="D979" s="3"/>
       <c r="E979" s="3"/>
       <c r="F979" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G979" s="3">
         <v>5000</v>
       </c>
       <c r="H979" s="3"/>
       <c r="I979" s="3" t="s">
-        <v>1803</v>
+        <v>1805</v>
       </c>
       <c r="J979" s="3" t="s">
-        <v>1804</v>
+        <v>1806</v>
       </c>
       <c r="X979" s="3"/>
     </row>
@@ -27705,17 +27721,17 @@
       <c r="D980" s="3"/>
       <c r="E980" s="3"/>
       <c r="F980" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G980" s="3">
         <v>5000</v>
       </c>
       <c r="H980" s="3"/>
       <c r="I980" s="3" t="s">
-        <v>1805</v>
+        <v>1807</v>
       </c>
       <c r="J980" s="3" t="s">
-        <v>1806</v>
+        <v>1808</v>
       </c>
       <c r="X980" s="3"/>
     </row>
@@ -27732,17 +27748,17 @@
       <c r="D981" s="3"/>
       <c r="E981" s="3"/>
       <c r="F981" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G981" s="3">
         <v>5000</v>
       </c>
       <c r="H981" s="3"/>
       <c r="I981" s="3" t="s">
-        <v>1807</v>
+        <v>1809</v>
       </c>
       <c r="J981" s="3" t="s">
-        <v>1808</v>
+        <v>1810</v>
       </c>
       <c r="X981" s="3"/>
     </row>
@@ -27759,17 +27775,17 @@
       <c r="D982" s="3"/>
       <c r="E982" s="3"/>
       <c r="F982" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G982" s="3">
         <v>5000</v>
       </c>
       <c r="H982" s="3"/>
       <c r="I982" s="3" t="s">
-        <v>1809</v>
+        <v>1811</v>
       </c>
       <c r="J982" s="3" t="s">
-        <v>1810</v>
+        <v>1812</v>
       </c>
       <c r="X982" s="3"/>
     </row>
@@ -27786,17 +27802,17 @@
       <c r="D983" s="3"/>
       <c r="E983" s="3"/>
       <c r="F983" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G983" s="3">
         <v>5000</v>
       </c>
       <c r="H983" s="3"/>
       <c r="I983" s="3" t="s">
-        <v>1811</v>
+        <v>1813</v>
       </c>
       <c r="J983" s="3" t="s">
-        <v>1812</v>
+        <v>1814</v>
       </c>
       <c r="X983" s="3"/>
     </row>
@@ -27813,17 +27829,17 @@
       <c r="D984" s="3"/>
       <c r="E984" s="3"/>
       <c r="F984" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G984" s="3">
         <v>5000</v>
       </c>
       <c r="H984" s="3"/>
       <c r="I984" s="3" t="s">
-        <v>1813</v>
+        <v>1815</v>
       </c>
       <c r="J984" s="3" t="s">
-        <v>1814</v>
+        <v>1816</v>
       </c>
       <c r="X984" s="3"/>
     </row>
@@ -27840,17 +27856,17 @@
       <c r="D985" s="3"/>
       <c r="E985" s="3"/>
       <c r="F985" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G985" s="3">
         <v>5000</v>
       </c>
       <c r="H985" s="3"/>
       <c r="I985" s="3" t="s">
-        <v>1815</v>
+        <v>1817</v>
       </c>
       <c r="J985" s="3" t="s">
-        <v>1816</v>
+        <v>1818</v>
       </c>
       <c r="X985" s="3"/>
     </row>
@@ -27867,17 +27883,17 @@
       <c r="D986" s="3"/>
       <c r="E986" s="3"/>
       <c r="F986" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G986" s="3">
         <v>5000</v>
       </c>
       <c r="H986" s="3"/>
       <c r="I986" s="3" t="s">
-        <v>1817</v>
+        <v>1819</v>
       </c>
       <c r="J986" s="3" t="s">
-        <v>1818</v>
+        <v>1820</v>
       </c>
       <c r="X986" s="3"/>
     </row>
@@ -27894,17 +27910,17 @@
       <c r="D987" s="3"/>
       <c r="E987" s="3"/>
       <c r="F987" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G987" s="3">
         <v>5000</v>
       </c>
       <c r="H987" s="3"/>
       <c r="I987" s="3" t="s">
-        <v>1819</v>
+        <v>1821</v>
       </c>
       <c r="J987" s="3" t="s">
-        <v>1820</v>
+        <v>1822</v>
       </c>
       <c r="X987" s="3"/>
     </row>
@@ -27921,17 +27937,17 @@
       <c r="D988" s="3"/>
       <c r="E988" s="3"/>
       <c r="F988" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G988" s="3">
         <v>1825</v>
       </c>
       <c r="H988" s="3"/>
       <c r="I988" s="3" t="s">
-        <v>1821</v>
+        <v>1823</v>
       </c>
       <c r="J988" s="3" t="s">
-        <v>1822</v>
+        <v>1824</v>
       </c>
       <c r="X988" s="3"/>
     </row>
@@ -27948,17 +27964,17 @@
       <c r="D989" s="3"/>
       <c r="E989" s="3"/>
       <c r="F989" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G989" s="3">
         <v>5000</v>
       </c>
       <c r="H989" s="3"/>
       <c r="I989" s="3" t="s">
-        <v>1823</v>
+        <v>1825</v>
       </c>
       <c r="J989" s="3" t="s">
-        <v>1824</v>
+        <v>1826</v>
       </c>
       <c r="X989" s="3"/>
     </row>
@@ -27975,17 +27991,17 @@
       <c r="D990" s="3"/>
       <c r="E990" s="3"/>
       <c r="F990" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G990" s="3">
         <v>5000</v>
       </c>
       <c r="H990" s="3"/>
       <c r="I990" s="3" t="s">
-        <v>1825</v>
+        <v>1827</v>
       </c>
       <c r="J990" s="3" t="s">
-        <v>1826</v>
+        <v>1828</v>
       </c>
       <c r="X990" s="3"/>
     </row>
@@ -28002,17 +28018,17 @@
       <c r="D991" s="3"/>
       <c r="E991" s="3"/>
       <c r="F991" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G991" s="3">
         <v>5000</v>
       </c>
       <c r="H991" s="3"/>
       <c r="I991" s="3" t="s">
-        <v>1827</v>
+        <v>1829</v>
       </c>
       <c r="J991" s="3" t="s">
-        <v>1828</v>
+        <v>1830</v>
       </c>
       <c r="X991" s="3"/>
     </row>
@@ -28029,17 +28045,17 @@
       <c r="D992" s="3"/>
       <c r="E992" s="3"/>
       <c r="F992" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G992" s="3">
         <v>5000</v>
       </c>
       <c r="H992" s="3"/>
       <c r="I992" s="3" t="s">
-        <v>1829</v>
+        <v>1831</v>
       </c>
       <c r="J992" s="3" t="s">
-        <v>1830</v>
+        <v>1832</v>
       </c>
       <c r="X992" s="3"/>
     </row>
@@ -28056,17 +28072,17 @@
       <c r="D993" s="3"/>
       <c r="E993" s="3"/>
       <c r="F993" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G993" s="3">
         <v>5000</v>
       </c>
       <c r="H993" s="3"/>
       <c r="I993" s="3" t="s">
-        <v>1831</v>
+        <v>1833</v>
       </c>
       <c r="J993" s="3" t="s">
-        <v>1832</v>
+        <v>1834</v>
       </c>
       <c r="X993" s="3"/>
     </row>
@@ -28083,17 +28099,17 @@
       <c r="D994" s="3"/>
       <c r="E994" s="3"/>
       <c r="F994" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G994" s="3">
         <v>5000</v>
       </c>
       <c r="H994" s="3"/>
       <c r="I994" s="3" t="s">
-        <v>1833</v>
+        <v>1835</v>
       </c>
       <c r="J994" s="3" t="s">
-        <v>1834</v>
+        <v>1836</v>
       </c>
       <c r="X994" s="3"/>
     </row>
@@ -28110,17 +28126,17 @@
       <c r="D995" s="3"/>
       <c r="E995" s="3"/>
       <c r="F995" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G995" s="3">
         <v>5000</v>
       </c>
       <c r="H995" s="3"/>
       <c r="I995" s="3" t="s">
-        <v>1835</v>
+        <v>1837</v>
       </c>
       <c r="J995" s="3" t="s">
-        <v>1836</v>
+        <v>1838</v>
       </c>
       <c r="X995" s="3"/>
     </row>
@@ -28137,17 +28153,17 @@
       <c r="D996" s="3"/>
       <c r="E996" s="3"/>
       <c r="F996" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G996" s="3">
         <v>5000</v>
       </c>
       <c r="H996" s="3"/>
       <c r="I996" s="3" t="s">
-        <v>1837</v>
+        <v>1839</v>
       </c>
       <c r="J996" s="3" t="s">
-        <v>1838</v>
+        <v>1840</v>
       </c>
       <c r="X996" s="3"/>
     </row>
@@ -28164,17 +28180,17 @@
       <c r="D997" s="3"/>
       <c r="E997" s="3"/>
       <c r="F997" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G997" s="3">
         <v>5000</v>
       </c>
       <c r="H997" s="3"/>
       <c r="I997" s="3" t="s">
-        <v>1839</v>
+        <v>1841</v>
       </c>
       <c r="J997" s="3" t="s">
-        <v>1840</v>
+        <v>1842</v>
       </c>
       <c r="X997" s="3"/>
     </row>
@@ -28191,17 +28207,17 @@
       <c r="D998" s="3"/>
       <c r="E998" s="3"/>
       <c r="F998" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G998" s="3">
         <v>5000</v>
       </c>
       <c r="H998" s="3"/>
       <c r="I998" s="3" t="s">
-        <v>1841</v>
+        <v>1843</v>
       </c>
       <c r="J998" s="3" t="s">
-        <v>1842</v>
+        <v>1844</v>
       </c>
       <c r="X998" s="3"/>
     </row>
@@ -28218,17 +28234,17 @@
       <c r="D999" s="3"/>
       <c r="E999" s="3"/>
       <c r="F999" s="3" t="s">
-        <v>1669</v>
+        <v>1671</v>
       </c>
       <c r="G999" s="3">
         <v>5000</v>
       </c>
       <c r="H999" s="3"/>
       <c r="I999" s="3" t="s">
-        <v>1843</v>
+        <v>1845</v>
       </c>
       <c r="J999" s="3" t="s">
-        <v>1844</v>
+        <v>1846</v>
       </c>
       <c r="X999" s="3"/>
     </row>
@@ -28840,8 +28856,128 @@
       <c r="J1031" s="3"/>
       <c r="X1031" s="3"/>
     </row>
+    <row r="1032" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F1032" s="3"/>
+      <c r="G1032" s="3"/>
+      <c r="H1032" s="3"/>
+      <c r="I1032" s="3"/>
+      <c r="J1032" s="3"/>
+      <c r="X1032" s="3"/>
+    </row>
+    <row r="1033" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F1033" s="3"/>
+      <c r="G1033" s="3"/>
+      <c r="H1033" s="3"/>
+      <c r="I1033" s="3"/>
+      <c r="J1033" s="3"/>
+      <c r="X1033" s="3"/>
+    </row>
+    <row r="1034" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F1034" s="3"/>
+      <c r="G1034" s="3"/>
+      <c r="H1034" s="3"/>
+      <c r="I1034" s="3"/>
+      <c r="J1034" s="3"/>
+      <c r="X1034" s="3"/>
+    </row>
+    <row r="1035" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F1035" s="3"/>
+      <c r="G1035" s="3"/>
+      <c r="H1035" s="3"/>
+      <c r="I1035" s="3"/>
+      <c r="J1035" s="3"/>
+      <c r="X1035" s="3"/>
+    </row>
+    <row r="1036" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F1036" s="3"/>
+      <c r="G1036" s="3"/>
+      <c r="H1036" s="3"/>
+      <c r="I1036" s="3"/>
+      <c r="J1036" s="3"/>
+      <c r="X1036" s="3"/>
+    </row>
+    <row r="1037" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F1037" s="3"/>
+      <c r="G1037" s="3"/>
+      <c r="H1037" s="3"/>
+      <c r="I1037" s="3"/>
+      <c r="J1037" s="3"/>
+      <c r="X1037" s="3"/>
+    </row>
+    <row r="1038" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F1038" s="3"/>
+      <c r="G1038" s="3"/>
+      <c r="H1038" s="3"/>
+      <c r="I1038" s="3"/>
+      <c r="J1038" s="3"/>
+      <c r="X1038" s="3"/>
+    </row>
+    <row r="1039" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F1039" s="3"/>
+      <c r="G1039" s="3"/>
+      <c r="H1039" s="3"/>
+      <c r="I1039" s="3"/>
+      <c r="J1039" s="3"/>
+      <c r="X1039" s="3"/>
+    </row>
+    <row r="1040" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F1040" s="3"/>
+      <c r="G1040" s="3"/>
+      <c r="H1040" s="3"/>
+      <c r="I1040" s="3"/>
+      <c r="J1040" s="3"/>
+      <c r="X1040" s="3"/>
+    </row>
+    <row r="1041" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F1041" s="3"/>
+      <c r="G1041" s="3"/>
+      <c r="H1041" s="3"/>
+      <c r="I1041" s="3"/>
+      <c r="J1041" s="3"/>
+      <c r="X1041" s="3"/>
+    </row>
+    <row r="1042" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F1042" s="3"/>
+      <c r="G1042" s="3"/>
+      <c r="H1042" s="3"/>
+      <c r="I1042" s="3"/>
+      <c r="J1042" s="3"/>
+      <c r="X1042" s="3"/>
+    </row>
+    <row r="1043" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F1043" s="3"/>
+      <c r="G1043" s="3"/>
+      <c r="H1043" s="3"/>
+      <c r="I1043" s="3"/>
+      <c r="J1043" s="3"/>
+      <c r="X1043" s="3"/>
+    </row>
+    <row r="1044" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F1044" s="3"/>
+      <c r="G1044" s="3"/>
+      <c r="H1044" s="3"/>
+      <c r="I1044" s="3"/>
+      <c r="J1044" s="3"/>
+      <c r="X1044" s="3"/>
+    </row>
+    <row r="1045" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F1045" s="3"/>
+      <c r="G1045" s="3"/>
+      <c r="H1045" s="3"/>
+      <c r="I1045" s="3"/>
+      <c r="J1045" s="3"/>
+      <c r="X1045" s="3"/>
+    </row>
+    <row r="1046" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F1046" s="3"/>
+      <c r="G1046" s="3"/>
+      <c r="H1046" s="3"/>
+      <c r="I1046" s="3"/>
+      <c r="J1046" s="3"/>
+      <c r="X1046" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="F1:J1031" xr:uid="{50090BFE-CB6D-4642-BA4B-F7E6AF828967}"/>
+  <autoFilter ref="F1:J1046" xr:uid="{50090BFE-CB6D-4642-BA4B-F7E6AF828967}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>